<commit_message>
Auto stash before rebase of "refs/heads/master"
</commit_message>
<xml_diff>
--- a/AOZ1281DI.xlsx
+++ b/AOZ1281DI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heinecke\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred\Downloads\SBC5-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D98764-DC01-43AA-B203-8A2E58BA2CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0D6E96-90B7-413D-9E74-F2C6D12CEC73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{D55AB5B1-4BC1-429F-82B8-F59F2B41C856}"/>
   </bookViews>
@@ -374,9 +374,9 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="0.000E+00"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="173" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -427,7 +427,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -716,6 +716,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -724,26 +737,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
@@ -756,15 +757,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="3" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="3" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="3" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -790,8 +791,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="3" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="3" fillId="3" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="3" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="3" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="8" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -801,33 +838,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="10" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="8" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -854,40 +873,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -943,6 +928,40 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -3319,14 +3338,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CFC006DC-B008-4A4E-AA27-302B054904D9}" name="Table2" displayName="Table2" ref="A73:F81" totalsRowShown="0" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CFC006DC-B008-4A4E-AA27-302B054904D9}" name="Table2" displayName="Table2" ref="A73:F81" totalsRowShown="0" tableBorderDxfId="9">
   <autoFilter ref="A73:F81" xr:uid="{4A76F8AC-30FC-48AB-B944-DEC569310B19}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CF3750E9-62E5-4A4E-A1A2-AC66A60CB49D}" name="Part number"/>
     <tableColumn id="2" xr3:uid="{9632C3C5-3C60-4B07-A1BE-20A4EABCF0CF}" name="Value"/>
     <tableColumn id="3" xr3:uid="{BE0EEA55-FC51-4E80-8ACA-578D9E3696A8}" name="Quantity"/>
     <tableColumn id="4" xr3:uid="{EF27F1FA-C129-4822-A127-F216B7281EE2}" name="Price/unit"/>
-    <tableColumn id="5" xr3:uid="{B4721B88-624D-4B67-890E-03CA1AA1958B}" name="Price" dataDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{B4721B88-624D-4B67-890E-03CA1AA1958B}" name="Price" dataDxfId="8" dataCellStyle="Currency">
       <calculatedColumnFormula>D74*C74</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{9A72E529-A5B4-4DCF-A857-F53DDAC6CE49}" name="Purpose"/>
@@ -3336,14 +3355,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F14AC3C4-D3B0-4392-B28C-49333C198959}" name="Table1" displayName="Table1" ref="A75:F83" totalsRowShown="0" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F14AC3C4-D3B0-4392-B28C-49333C198959}" name="Table1" displayName="Table1" ref="A75:F83" totalsRowShown="0" tableBorderDxfId="1">
   <autoFilter ref="A75:F83" xr:uid="{EB5E68EE-CBD9-4C56-AA00-C93F9EBD892A}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{4E26CB2C-D447-4F24-AF3E-EED540EF7026}" name="Part number"/>
     <tableColumn id="2" xr3:uid="{37C3BFF4-D988-49F4-90C8-412925F683D8}" name="Value"/>
     <tableColumn id="3" xr3:uid="{B54A28A7-C6D7-42A7-9475-6EAA259F41CE}" name="Quantity"/>
     <tableColumn id="4" xr3:uid="{490048DC-F491-4B3B-9B4F-80E7EE88E6A1}" name="Price/unit"/>
-    <tableColumn id="5" xr3:uid="{44D7CBAB-E8E8-4CF5-B9B7-6D2EBA64816F}" name="Price" dataDxfId="1" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{44D7CBAB-E8E8-4CF5-B9B7-6D2EBA64816F}" name="Price" dataDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>D76*C76</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{957B4911-2007-4EAD-A0FF-C82F5429E22B}" name="Purpose"/>
@@ -3682,719 +3701,719 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="33" t="s">
+      <c r="F2" s="65"/>
+      <c r="G2" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19">
+      <c r="A4" s="15">
         <v>0.8</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="16">
         <v>5</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="16">
         <v>12</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="16">
         <v>1</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="16">
         <v>1200000</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="16">
         <v>1800000</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="26">
         <f>F4*0.0000001</f>
         <v>0.18</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="57"/>
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="34" t="s">
+      <c r="K7" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="32" t="s">
+      <c r="L7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="37" t="s">
+      <c r="M7" s="33" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
+      <c r="A8" s="23">
         <v>1E-3</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="16">
         <v>147000</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="24">
         <f>A4*B8/(B4-A4)</f>
         <v>28000</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="11">
         <f>B8*(1-A8)</f>
         <v>146853</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="11">
         <f>B8*(1+A8)</f>
         <v>147146.99999999997</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="20">
         <f>C8*(1-A8)</f>
         <v>27972</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="20">
         <f>C8*(1+A8)</f>
         <v>28027.999999999996</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="21">
         <f>A4*(1+D8/G8)</f>
         <v>4.9916083916083922</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="21">
         <f>A4*(1+B8/C8)</f>
         <v>5</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="21">
         <f>A4*(1+E8/F8)</f>
         <v>5.0084084084084077</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="21">
         <f>ABS(MAX(J8, H8)-B4)</f>
         <v>8.4084084084077304E-3</v>
       </c>
-      <c r="L8" s="29">
+      <c r="L8" s="25">
         <f>K8/B4</f>
         <v>1.681681681681546E-3</v>
       </c>
-      <c r="M8" s="40">
+      <c r="M8" s="36">
         <f>J8^2/(E8+F8)</f>
         <v>1.4324062372110419E-4</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="8"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="57"/>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="34" t="s">
+      <c r="I11" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="K11" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="L11" s="32" t="s">
+      <c r="L11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="37" t="s">
+      <c r="M11" s="33" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+      <c r="A12" s="23">
         <v>1E-3</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="16">
         <f>B8</f>
         <v>147000</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="19">
         <v>28000</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="11">
         <f>B12*(1-A12)</f>
         <v>146853</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="11">
         <f>B12*(1+A12)</f>
         <v>147146.99999999997</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="20">
         <f>C12*(1-A12)</f>
         <v>27972</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="20">
         <f>C12*(1+A12)</f>
         <v>28027.999999999996</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="21">
         <f>A4*(1+D12/G12)</f>
         <v>4.9916083916083922</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="21">
         <f>A4*(1+B12/C12)</f>
         <v>5</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="21">
         <f>A4*(1+E12/F12)</f>
         <v>5.0084084084084077</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="21">
         <f>ABS(MAX(J12, H12)-B4)</f>
         <v>8.4084084084077304E-3</v>
       </c>
-      <c r="L12" s="26">
+      <c r="L12" s="22">
         <f>K12/B4</f>
         <v>1.681681681681546E-3</v>
       </c>
-      <c r="M12" s="40">
+      <c r="M12" s="36">
         <f>J12*J12/(E12+F12)</f>
         <v>1.4324062372110419E-4</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="E14" s="6" t="s">
+      <c r="B14" s="56"/>
+      <c r="C14" s="57"/>
+      <c r="E14" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="33" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19">
+      <c r="A16" s="15">
         <v>0.01</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="17">
         <f>(D4/(E4*A16))*(1-B4/C4)*(B4/C4)</f>
         <v>2.0254629629629626E-5</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="37">
         <f>D4*SQRT((B4/C4)*(1-B4/C4))</f>
         <v>0.49300664859163462</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="22">
+      <c r="E16" s="18">
         <v>1.1E-4</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="21">
         <f>(D4/(E4*E16))*(1-B4/C4)*(B4/C4)</f>
         <v>1.8413299663299664E-3</v>
       </c>
-      <c r="G16" s="44">
+      <c r="G16" s="37">
         <f>D4*SQRT((B4/C4)*(1-B4/C4))</f>
         <v>0.49300664859163462</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="E18" s="6" t="s">
+      <c r="B18" s="56"/>
+      <c r="C18" s="57"/>
+      <c r="E18" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="57"/>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="33" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19">
+      <c r="A20" s="15">
         <v>0.01</v>
       </c>
-      <c r="B20" s="39">
+      <c r="B20" s="35">
         <f>(B4/(E4*A20))*(1-B4/C4)</f>
         <v>2.4305555555555555E-4</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="13">
         <f>D4+A20/2</f>
         <v>1.0049999999999999</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="15">
         <v>2.2000000000000001E-4</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="21">
         <f>(B4/(E4*E20))*(1-B4/C4)</f>
         <v>1.1047979797979796E-2</v>
       </c>
-      <c r="G20" s="44">
+      <c r="G20" s="37">
         <f>D4+F20/2</f>
         <v>1.0055239898989898</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="63"/>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19">
+      <c r="A24" s="15">
         <v>0.01</v>
       </c>
-      <c r="B24" s="46">
+      <c r="B24" s="39">
         <v>0.125</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24" s="21">
         <f>B24/(2*PI()*E4*A20/(8*E4*A24))</f>
         <v>0.15915494309189535</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="17">
         <f>A20/(8*E4*(A24-A20*C24))</f>
         <v>1.2388330740707554E-7</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="21">
         <f>A20/SQRT(12)</f>
         <v>2.886751345948129E-3</v>
       </c>
-      <c r="F24" s="44">
+      <c r="F24" s="37">
         <f>A24+B4</f>
         <v>5.01</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="63"/>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="37" t="s">
+      <c r="F27" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="45">
+      <c r="A28" s="38">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="B28" s="46">
+      <c r="B28" s="39">
         <v>0.125</v>
       </c>
-      <c r="C28" s="47">
+      <c r="C28" s="40">
         <f>B28/(2*PI()*E4*A28)</f>
         <v>1.6578639905405763E-2</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="21">
         <f>F20*(C28+1/(8*E4*A28))</f>
         <v>1.3339917077091336E-3</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="21">
         <f>F20/SQRT(12)</f>
         <v>3.1892770551825915E-3</v>
       </c>
-      <c r="F28" s="44">
+      <c r="F28" s="37">
         <f>D28+J12</f>
         <v>5.0097424001161173</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57"/>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="37" t="s">
+      <c r="F31" s="33" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="19">
+      <c r="A32" s="15">
         <v>0.5</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B32" s="16">
         <v>20</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="16">
         <v>2</v>
       </c>
-      <c r="D32" s="20">
+      <c r="D32" s="16">
         <v>80</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="11">
         <f>D4*(1-G4)*A32</f>
         <v>0.41000000000000003</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F32" s="13">
         <f>E32*D32</f>
         <v>32.800000000000004</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="8"/>
+      <c r="B34" s="57"/>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="33" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="19">
+      <c r="A36" s="15">
         <v>0.38</v>
       </c>
-      <c r="B36" s="44">
+      <c r="B36" s="37">
         <f>1.1*G20^2*A36</f>
         <v>0.42263081060167651</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="34" t="s">
+      <c r="E39" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="34" t="s">
+      <c r="F39" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G39" s="37" t="s">
+      <c r="G39" s="33" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="18">
+      <c r="A40" s="14">
         <f>0.38+(C4-3.3)*(0.24-0.38)/(12-3.3)</f>
         <v>0.24</v>
       </c>
-      <c r="B40" s="25">
+      <c r="B40" s="21">
         <f>G20^2*A40</f>
         <v>0.24265883862297211</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C40" s="11">
         <v>1.5E-3</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="11">
         <f>C40*C4</f>
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="E40" s="25">
+      <c r="E40" s="21">
         <f>D40+B40</f>
         <v>0.26065883862297212</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="11">
         <v>55</v>
       </c>
-      <c r="G40" s="17">
+      <c r="G40" s="13">
         <f>F40*E40</f>
         <v>14.336236124263467</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="57"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="C43" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="37" t="s">
+      <c r="D43" s="33" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="51">
+      <c r="A44" s="44">
         <f>E40+B36+E32+M12</f>
         <v>1.0934328898483698</v>
       </c>
-      <c r="B44" s="25">
+      <c r="B44" s="21">
         <f>B4*D4+A44</f>
         <v>6.0934328898483701</v>
       </c>
-      <c r="C44" s="50">
+      <c r="C44" s="43">
         <f>B4*D4/B44</f>
         <v>0.82055552106432095</v>
       </c>
-      <c r="D44" s="44">
+      <c r="D44" s="37">
         <f>B44/C4</f>
         <v>0.50778607415403088</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="57"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -4402,287 +4421,287 @@
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="33" t="s">
+      <c r="C47" s="29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="11">
+      <c r="A48" s="5"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="7">
         <f>C44</f>
         <v>0.82055552106432095</v>
       </c>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+      <c r="A49" s="5">
         <v>-20</v>
       </c>
-      <c r="B49" s="48">
+      <c r="B49" s="41">
         <f>10^(A49/10)</f>
         <v>0.01</v>
       </c>
-      <c r="C49" s="11">
+      <c r="C49" s="7">
         <f t="dataTable" ref="C49:C70" dt2D="0" dtr="0" r1="D4"/>
         <v>0.69059042379965763</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+      <c r="A50" s="5">
         <v>-19</v>
       </c>
-      <c r="B50" s="48">
+      <c r="B50" s="41">
         <f t="shared" ref="B50:B70" si="0">10^(A50/10)</f>
         <v>1.2589254117941664E-2</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="7">
         <v>0.72798037471181143</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
+      <c r="A51" s="5">
         <v>-18</v>
       </c>
-      <c r="B51" s="48">
+      <c r="B51" s="41">
         <f t="shared" si="0"/>
         <v>1.5848931924611124E-2</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="7">
         <v>0.76060363662403097</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+      <c r="A52" s="5">
         <v>-17</v>
       </c>
-      <c r="B52" s="48">
+      <c r="B52" s="41">
         <f t="shared" si="0"/>
         <v>1.9952623149688792E-2</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="7">
         <v>0.78855388622133216</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="9">
+      <c r="A53" s="5">
         <v>-16</v>
       </c>
-      <c r="B53" s="48">
+      <c r="B53" s="41">
         <f t="shared" si="0"/>
         <v>2.511886431509578E-2</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="7">
         <v>0.81209798050687554</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
+      <c r="A54" s="5">
         <v>-15</v>
       </c>
-      <c r="B54" s="48">
+      <c r="B54" s="41">
         <f t="shared" si="0"/>
         <v>3.1622776601683784E-2</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="7">
         <v>0.83160747875367458</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
+      <c r="A55" s="5">
         <v>-14</v>
       </c>
-      <c r="B55" s="48">
+      <c r="B55" s="41">
         <f t="shared" si="0"/>
         <v>3.9810717055349727E-2</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="7">
         <v>0.84749971890299669</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+      <c r="A56" s="5">
         <v>-13</v>
       </c>
-      <c r="B56" s="48">
+      <c r="B56" s="41">
         <f t="shared" si="0"/>
         <v>5.0118723362727206E-2</v>
       </c>
-      <c r="C56" s="11">
+      <c r="C56" s="7">
         <v>0.86019232949422586</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="9">
+      <c r="A57" s="5">
         <v>-12</v>
       </c>
-      <c r="B57" s="48">
+      <c r="B57" s="41">
         <f t="shared" si="0"/>
         <v>6.3095734448019317E-2</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="7">
         <v>0.87007125498392679</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
+      <c r="A58" s="5">
         <v>-11</v>
       </c>
-      <c r="B58" s="48">
+      <c r="B58" s="41">
         <f t="shared" si="0"/>
         <v>7.9432823472428096E-2</v>
       </c>
-      <c r="C58" s="11">
+      <c r="C58" s="7">
         <v>0.87747023089874654</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="9">
+      <c r="A59" s="5">
         <v>-10</v>
       </c>
-      <c r="B59" s="48">
+      <c r="B59" s="41">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="C59" s="11">
+      <c r="C59" s="7">
         <v>0.8826588454799541</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="9">
+      <c r="A60" s="5">
         <v>-9</v>
       </c>
-      <c r="B60" s="48">
+      <c r="B60" s="41">
         <f t="shared" si="0"/>
         <v>0.12589254117941667</v>
       </c>
-      <c r="C60" s="11">
+      <c r="C60" s="7">
         <v>0.88583637781754987</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="9">
+      <c r="A61" s="5">
         <v>-8</v>
       </c>
-      <c r="B61" s="48">
+      <c r="B61" s="41">
         <f t="shared" si="0"/>
         <v>0.15848931924611132</v>
       </c>
-      <c r="C61" s="11">
+      <c r="C61" s="7">
         <v>0.88712908675677771</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="9">
+      <c r="A62" s="5">
         <v>-7</v>
       </c>
-      <c r="B62" s="48">
+      <c r="B62" s="41">
         <f t="shared" si="0"/>
         <v>0.19952623149688795</v>
       </c>
-      <c r="C62" s="11">
+      <c r="C62" s="7">
         <v>0.88658926267951899</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="9">
+      <c r="A63" s="5">
         <v>-6</v>
       </c>
-      <c r="B63" s="48">
+      <c r="B63" s="41">
         <f t="shared" si="0"/>
         <v>0.25118864315095801</v>
       </c>
-      <c r="C63" s="11">
+      <c r="C63" s="7">
         <v>0.88419500431857101</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="9">
+      <c r="A64" s="5">
         <v>-5</v>
       </c>
-      <c r="B64" s="48">
+      <c r="B64" s="41">
         <f t="shared" si="0"/>
         <v>0.31622776601683794</v>
       </c>
-      <c r="C64" s="11">
+      <c r="C64" s="7">
         <v>0.87985030029745082</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="9">
+      <c r="A65" s="5">
         <v>-4</v>
       </c>
-      <c r="B65" s="48">
+      <c r="B65" s="41">
         <f t="shared" si="0"/>
         <v>0.3981071705534972</v>
       </c>
-      <c r="C65" s="11">
+      <c r="C65" s="7">
         <v>0.87338559069235189</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="9">
+      <c r="A66" s="5">
         <v>-3</v>
       </c>
-      <c r="B66" s="48">
+      <c r="B66" s="41">
         <f t="shared" si="0"/>
         <v>0.50118723362727224</v>
       </c>
-      <c r="C66" s="11">
+      <c r="C66" s="7">
         <v>0.86455958928421106</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
+      <c r="A67" s="5">
         <v>-2</v>
       </c>
-      <c r="B67" s="48">
+      <c r="B67" s="41">
         <f t="shared" si="0"/>
         <v>0.63095734448019325</v>
       </c>
-      <c r="C67" s="11">
+      <c r="C67" s="7">
         <v>0.85306378530717675</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="9">
+      <c r="A68" s="5">
         <v>-1</v>
       </c>
-      <c r="B68" s="48">
+      <c r="B68" s="41">
         <f t="shared" si="0"/>
         <v>0.79432823472428149</v>
       </c>
-      <c r="C68" s="11">
+      <c r="C68" s="7">
         <v>0.83853169694160123</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
+      <c r="A69" s="5">
         <v>0</v>
       </c>
-      <c r="B69" s="48">
+      <c r="B69" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C69" s="11">
+      <c r="C69" s="7">
         <v>0.82055552106432095</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="12">
+      <c r="A70" s="8">
         <v>1</v>
       </c>
-      <c r="B70" s="49">
+      <c r="B70" s="42">
         <f t="shared" si="0"/>
         <v>1.2589254117941673</v>
       </c>
-      <c r="C70" s="14">
+      <c r="C70" s="10">
         <v>0.79871309698574922</v>
       </c>
     </row>
@@ -4690,225 +4709,233 @@
       <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="61" t="s">
+      <c r="A72" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="62"/>
-      <c r="C72" s="62"/>
-      <c r="D72" s="62"/>
-      <c r="E72" s="62"/>
-      <c r="F72" s="63"/>
+      <c r="B72" s="59"/>
+      <c r="C72" s="59"/>
+      <c r="D72" s="59"/>
+      <c r="E72" s="59"/>
+      <c r="F72" s="60"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="53" t="s">
+      <c r="A73" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="B73" s="54" t="s">
+      <c r="B73" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="C73" s="54" t="s">
+      <c r="C73" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="D73" s="54" t="s">
+      <c r="D73" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E73" s="54" t="s">
+      <c r="E73" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="F73" s="55" t="s">
+      <c r="F73" s="48" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="53" t="s">
+      <c r="A74" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="B74" s="54" t="s">
+      <c r="B74" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="C74" s="54">
+      <c r="C74" s="47">
         <v>1</v>
       </c>
-      <c r="D74" s="54">
+      <c r="D74" s="47">
         <v>0.31</v>
       </c>
-      <c r="E74" s="56">
+      <c r="E74" s="49">
         <f>D74*C74</f>
         <v>0.31</v>
       </c>
-      <c r="F74" s="55" t="s">
+      <c r="F74" s="48" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="53" t="s">
+      <c r="A75" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="54" t="s">
+      <c r="B75" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="54">
+      <c r="C75" s="47">
         <v>1</v>
       </c>
-      <c r="D75" s="54">
+      <c r="D75" s="47">
         <v>0.23</v>
       </c>
-      <c r="E75" s="56">
+      <c r="E75" s="49">
         <f>D75*C75</f>
         <v>0.23</v>
       </c>
-      <c r="F75" s="55" t="s">
+      <c r="F75" s="48" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="57" t="s">
+      <c r="A76" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="B76" s="54" t="s">
+      <c r="B76" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="C76" s="54">
+      <c r="C76" s="47">
         <v>1</v>
       </c>
-      <c r="D76" s="54">
+      <c r="D76" s="47">
         <v>0.42</v>
       </c>
-      <c r="E76" s="56">
+      <c r="E76" s="49">
         <f t="shared" ref="E76:E81" si="1">D76*C76</f>
         <v>0.42</v>
       </c>
-      <c r="F76" s="55" t="s">
+      <c r="F76" s="48" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="53" t="s">
+      <c r="A77" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B77" s="54" t="s">
+      <c r="B77" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C77" s="54">
+      <c r="C77" s="47">
         <v>1</v>
       </c>
-      <c r="D77" s="54">
+      <c r="D77" s="47">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E77" s="56">
+      <c r="E77" s="49">
         <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
-      <c r="F77" s="55" t="s">
+      <c r="F77" s="48" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="53" t="s">
+      <c r="A78" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="54"/>
-      <c r="C78" s="54">
+      <c r="B78" s="47"/>
+      <c r="C78" s="47">
         <v>1</v>
       </c>
-      <c r="D78" s="54">
+      <c r="D78" s="47">
         <v>0.69299999999999995</v>
       </c>
-      <c r="E78" s="56">
+      <c r="E78" s="49">
         <f t="shared" si="1"/>
         <v>0.69299999999999995</v>
       </c>
-      <c r="F78" s="55" t="s">
+      <c r="F78" s="48" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="53" t="s">
+      <c r="A79" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B79" s="54" t="s">
+      <c r="B79" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="C79" s="54">
+      <c r="C79" s="47">
         <v>1</v>
       </c>
-      <c r="D79" s="54">
+      <c r="D79" s="47">
         <v>1.1599999999999999</v>
       </c>
-      <c r="E79" s="56">
+      <c r="E79" s="49">
         <f t="shared" si="1"/>
         <v>1.1599999999999999</v>
       </c>
-      <c r="F79" s="55" t="s">
+      <c r="F79" s="48" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="53" t="s">
+      <c r="A80" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="B80" s="54" t="s">
+      <c r="B80" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="C80" s="54">
+      <c r="C80" s="47">
         <v>1</v>
       </c>
-      <c r="D80" s="54">
+      <c r="D80" s="47">
         <v>0.1</v>
       </c>
-      <c r="E80" s="56">
+      <c r="E80" s="49">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F80" s="55" t="s">
+      <c r="F80" s="48" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="53" t="s">
+      <c r="A81" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B81" s="54"/>
-      <c r="C81" s="54">
+      <c r="B81" s="47"/>
+      <c r="C81" s="47">
         <v>1</v>
       </c>
-      <c r="D81" s="54">
+      <c r="D81" s="47">
         <v>0.16</v>
       </c>
-      <c r="E81" s="60">
+      <c r="E81" s="53">
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-      <c r="F81" s="55" t="s">
+      <c r="F81" s="48" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="53"/>
-      <c r="B82" s="54"/>
-      <c r="C82" s="54"/>
-      <c r="D82" s="54"/>
-      <c r="E82" s="54"/>
-      <c r="F82" s="55"/>
+      <c r="A82" s="46"/>
+      <c r="B82" s="47"/>
+      <c r="C82" s="47"/>
+      <c r="D82" s="47"/>
+      <c r="E82" s="47"/>
+      <c r="F82" s="48"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="58"/>
-      <c r="B83" s="13" t="s">
+      <c r="A83" s="51"/>
+      <c r="B83" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C83" s="13">
+      <c r="C83" s="9">
         <f>SUM(Table2[Quantity])</f>
         <v>8</v>
       </c>
-      <c r="D83" s="13"/>
-      <c r="E83" s="64">
+      <c r="D83" s="9"/>
+      <c r="E83" s="54">
         <f>SUM(Table2[Price])</f>
         <v>3.363</v>
       </c>
-      <c r="F83" s="59"/>
+      <c r="F83" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="E18:G18"/>
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A72:F72"/>
@@ -4917,14 +4944,6 @@
     <mergeCell ref="A30:F30"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A6:M6"/>
   </mergeCells>
   <conditionalFormatting sqref="G40">
     <cfRule type="colorScale" priority="1">
@@ -4973,8 +4992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5CAF6-20E4-4B67-AE88-D57C6FEB2845}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5003,719 +5022,719 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="33" t="s">
+      <c r="F2" s="65"/>
+      <c r="G2" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19">
+      <c r="A4" s="15">
         <v>0.8</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="16">
         <v>3.7</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="16">
         <v>12</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="16">
         <v>1.4950000000000001</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="16">
         <v>1200000</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="16">
         <v>1800000</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="26">
         <f>F4*0.0000001</f>
         <v>0.18</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="57"/>
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="34" t="s">
+      <c r="K7" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="32" t="s">
+      <c r="L7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="37" t="s">
+      <c r="M7" s="33" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
+      <c r="A8" s="23">
         <v>1E-3</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="16">
         <v>49900</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="24">
         <f>A4*B8/(B4-A4)</f>
         <v>13765.517241379308</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="11">
         <f>B8*(1-A8)</f>
         <v>49850.1</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="11">
         <f>B8*(1+A8)</f>
         <v>49949.899999999994</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="20">
         <f>C8*(1-A8)</f>
         <v>13751.751724137928</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="20">
         <f>C8*(1+A8)</f>
         <v>13779.282758620686</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="21">
         <f>A4*(1+D8/G8)</f>
         <v>3.6942057942057951</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="21">
         <f>A4*(1+B8/C8)</f>
         <v>3.7</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="21">
         <f>A4*(1+E8/F8)</f>
         <v>3.7058058058058068</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="21">
         <f>ABS(MAX(J8, H8)-B4)</f>
         <v>5.8058058058065853E-3</v>
       </c>
-      <c r="L8" s="29">
+      <c r="L8" s="25">
         <f>K8/B4</f>
         <v>1.56913670427205E-3</v>
       </c>
-      <c r="M8" s="40">
+      <c r="M8" s="36">
         <f>J8^2/(E8+F8)</f>
         <v>2.1558305473483194E-4</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="8"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="57"/>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="34" t="s">
+      <c r="I11" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="K11" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="L11" s="32" t="s">
+      <c r="L11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="37" t="s">
+      <c r="M11" s="33" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+      <c r="A12" s="23">
         <v>1E-3</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="16">
         <f>B8</f>
         <v>49900</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="19">
         <v>13700</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="11">
         <f>B12*(1-A12)</f>
         <v>49850.1</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="11">
         <f>B12*(1+A12)</f>
         <v>49949.899999999994</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="20">
         <f>C12*(1-A12)</f>
         <v>13686.3</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="20">
         <f>C12*(1+A12)</f>
         <v>13713.699999999999</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="21">
         <f>A4*(1+D12/G12)</f>
         <v>3.7080466978277205</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="21">
         <f>A4*(1+B12/C12)</f>
         <v>3.7138686131386862</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="21">
         <f>A4*(1+E12/F12)</f>
         <v>3.7197021839357607</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="21">
         <f>ABS(MAX(J12, H12)-B4)</f>
         <v>1.9702183935760509E-2</v>
       </c>
-      <c r="L12" s="26">
+      <c r="L12" s="22">
         <f>K12/B4</f>
         <v>5.3249145772325699E-3</v>
       </c>
-      <c r="M12" s="40">
+      <c r="M12" s="36">
         <f>J12*J12/(E12+F12)</f>
         <v>2.1742631296614928E-4</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="E14" s="6" t="s">
+      <c r="B14" s="56"/>
+      <c r="C14" s="57"/>
+      <c r="E14" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="66" t="s">
         <v>43</v>
       </c>
       <c r="F15" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="33" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19">
+      <c r="A16" s="15">
         <v>0.01</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="17">
         <f>(D4/(E4*A16))*(1-B4/C4)*(B4/C4)</f>
         <v>2.6569126157407413E-5</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="37">
         <f>D4*SQRT((B4/C4)*(1-B4/C4))</f>
         <v>0.69039852495778764</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="22">
+      <c r="E16" s="18">
         <v>1.1E-4</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="21">
         <f>(D4/(E4*E16))*(1-B4/C4)*(B4/C4)</f>
         <v>2.4153751052188553E-3</v>
       </c>
-      <c r="G16" s="44">
+      <c r="G16" s="37">
         <f>D4*SQRT((B4/C4)*(1-B4/C4))</f>
         <v>0.69039852495778764</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="E18" s="6" t="s">
+      <c r="B18" s="56"/>
+      <c r="C18" s="57"/>
+      <c r="E18" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="57"/>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="33" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19">
+      <c r="A20" s="15">
         <v>0.01</v>
       </c>
-      <c r="B20" s="39">
+      <c r="B20" s="35">
         <f>(B4/(E4*A20))*(1-B4/C4)</f>
         <v>2.1326388888888889E-4</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="13">
         <f>D4+A20/2</f>
         <v>1.5</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="15">
         <v>2.2000000000000001E-4</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="21">
         <f>(B4/(E4*E20))*(1-B4/C4)</f>
         <v>9.6938131313131313E-3</v>
       </c>
-      <c r="G20" s="44">
+      <c r="G20" s="37">
         <f>D4+F20/2</f>
         <v>1.4998469065656568</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="63"/>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19">
+      <c r="A24" s="15">
         <v>0.01</v>
       </c>
-      <c r="B24" s="52">
+      <c r="B24" s="45">
         <v>0.125</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24" s="21">
         <f>B24/(2*PI()*E4*A20/(8*E4*A24))</f>
         <v>0.15915494309189535</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="11">
         <f>A20/(8*E4*(A24-A20*C24))</f>
         <v>1.2388330740707554E-7</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="21">
         <f>A20/SQRT(12)</f>
         <v>2.886751345948129E-3</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="13">
         <f>A24+B4</f>
         <v>3.71</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="63"/>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="37" t="s">
+      <c r="F27" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="45">
+      <c r="A28" s="38">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="B28" s="52">
+      <c r="B28" s="45">
         <v>0.125</v>
       </c>
-      <c r="C28" s="47">
+      <c r="C28" s="40">
         <f>B28/(2*PI()*E4*A28)</f>
         <v>1.6578639905405763E-2</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="21">
         <f>F20*(C28+1/(8*E4*A28))</f>
         <v>1.1704824383927856E-3</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="21">
         <f>F20/SQRT(12)</f>
         <v>2.7983628104187828E-3</v>
       </c>
-      <c r="F28" s="44">
+      <c r="F28" s="37">
         <f>D28+J12</f>
         <v>3.7208726663741536</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57"/>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="37" t="s">
+      <c r="F31" s="33" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="19">
+      <c r="A32" s="15">
         <v>0.5</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B32" s="16">
         <v>20</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="16">
         <v>2</v>
       </c>
-      <c r="D32" s="20">
+      <c r="D32" s="16">
         <v>80</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="21">
         <f>D4*(1-G4)*A32</f>
         <v>0.61295000000000011</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F32" s="13">
         <f>E32*D32</f>
         <v>49.036000000000008</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="8"/>
+      <c r="B34" s="57"/>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="33" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="19">
+      <c r="A36" s="15">
         <v>0.315</v>
       </c>
-      <c r="B36" s="44">
+      <c r="B36" s="37">
         <f>1.1*G20^2*A36</f>
         <v>0.77946586749612856</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="34" t="s">
+      <c r="E39" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="34" t="s">
+      <c r="F39" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G39" s="37" t="s">
+      <c r="G39" s="33" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="18">
+      <c r="A40" s="14">
         <f>0.38+(C4-3.3)*(0.24-0.38)/(12-3.3)</f>
         <v>0.24</v>
       </c>
-      <c r="B40" s="25">
+      <c r="B40" s="21">
         <f>G20^2*A40</f>
         <v>0.53988977835229679</v>
       </c>
-      <c r="C40" s="25">
+      <c r="C40" s="21">
         <v>1.5E-3</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="11">
         <f>C40*C4</f>
         <v>1.8000000000000002E-2</v>
       </c>
-      <c r="E40" s="25">
+      <c r="E40" s="21">
         <f>D40+B40</f>
         <v>0.55788977835229681</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="11">
         <v>55</v>
       </c>
-      <c r="G40" s="17">
+      <c r="G40" s="13">
         <f>F40*E40</f>
         <v>30.683937809376324</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="57"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="C43" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="37" t="s">
+      <c r="D43" s="33" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="51">
+      <c r="A44" s="44">
         <f>E40+B36+E32+M12</f>
         <v>1.9505230721613918</v>
       </c>
-      <c r="B44" s="25">
+      <c r="B44" s="21">
         <f>B4*D4+A44</f>
         <v>7.4820230721613923</v>
       </c>
-      <c r="C44" s="16">
+      <c r="C44" s="12">
         <f>B4*D4/B44</f>
         <v>0.73930539195758871</v>
       </c>
-      <c r="D44" s="44">
+      <c r="D44" s="37">
         <f>B44/C4</f>
         <v>0.62350192268011606</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="57"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -5723,311 +5742,311 @@
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="33" t="s">
+      <c r="C47" s="29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="11">
+      <c r="A48" s="5"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="7">
         <f>C44</f>
         <v>0.73930539195758871</v>
       </c>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+      <c r="A49" s="5">
         <v>-20</v>
       </c>
-      <c r="B49" s="48">
+      <c r="B49" s="41">
         <f>10^(A49/10)</f>
         <v>0.01</v>
       </c>
-      <c r="C49" s="11">
+      <c r="C49" s="7">
         <f t="dataTable" ref="C49:C72" dt2D="0" dtr="0" r1="D4"/>
         <v>0.62240619702935862</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+      <c r="A50" s="5">
         <v>-19</v>
       </c>
-      <c r="B50" s="48">
+      <c r="B50" s="41">
         <f t="shared" ref="B50:B72" si="0">10^(A50/10)</f>
         <v>1.2589254117941664E-2</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="7">
         <v>0.66412682063428197</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
+      <c r="A51" s="5">
         <v>-18</v>
       </c>
-      <c r="B51" s="48">
+      <c r="B51" s="41">
         <f t="shared" si="0"/>
         <v>1.5848931924611124E-2</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="7">
         <v>0.70138296650231557</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+      <c r="A52" s="5">
         <v>-17</v>
       </c>
-      <c r="B52" s="48">
+      <c r="B52" s="41">
         <f t="shared" si="0"/>
         <v>1.9952623149688792E-2</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="7">
         <v>0.73396499657999337</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="9">
+      <c r="A53" s="5">
         <v>-16</v>
       </c>
-      <c r="B53" s="48">
+      <c r="B53" s="41">
         <f t="shared" si="0"/>
         <v>2.511886431509578E-2</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="7">
         <v>0.76191025850561611</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
+      <c r="A54" s="5">
         <v>-15</v>
       </c>
-      <c r="B54" s="48">
+      <c r="B54" s="41">
         <f t="shared" si="0"/>
         <v>3.1622776601683784E-2</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="7">
         <v>0.78543698075365709</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
+      <c r="A55" s="5">
         <v>-14</v>
       </c>
-      <c r="B55" s="48">
+      <c r="B55" s="41">
         <f t="shared" si="0"/>
         <v>3.9810717055349727E-2</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="7">
         <v>0.80487597113032094</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+      <c r="A56" s="5">
         <v>-13</v>
       </c>
-      <c r="B56" s="48">
+      <c r="B56" s="41">
         <f t="shared" si="0"/>
         <v>5.0118723362727206E-2</v>
       </c>
-      <c r="C56" s="11">
+      <c r="C56" s="7">
         <v>0.82061010469092444</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="9">
+      <c r="A57" s="5">
         <v>-12</v>
       </c>
-      <c r="B57" s="48">
+      <c r="B57" s="41">
         <f t="shared" si="0"/>
         <v>6.3095734448019317E-2</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="7">
         <v>0.83302635349491971</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
+      <c r="A58" s="5">
         <v>-11</v>
       </c>
-      <c r="B58" s="48">
+      <c r="B58" s="41">
         <f t="shared" si="0"/>
         <v>7.9432823472428096E-2</v>
       </c>
-      <c r="C58" s="11">
+      <c r="C58" s="7">
         <v>0.8424810761986421</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="9">
+      <c r="A59" s="5">
         <v>-10</v>
       </c>
-      <c r="B59" s="48">
+      <c r="B59" s="41">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="C59" s="11">
+      <c r="C59" s="7">
         <v>0.84927688713019533</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="9">
+      <c r="A60" s="5">
         <v>-9</v>
       </c>
-      <c r="B60" s="48">
+      <c r="B60" s="41">
         <f t="shared" si="0"/>
         <v>0.12589254117941667</v>
       </c>
-      <c r="C60" s="11">
+      <c r="C60" s="7">
         <v>0.85364843514519362</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="9">
+      <c r="A61" s="5">
         <v>-8</v>
       </c>
-      <c r="B61" s="48">
+      <c r="B61" s="41">
         <f t="shared" si="0"/>
         <v>0.15848931924611132</v>
       </c>
-      <c r="C61" s="11">
+      <c r="C61" s="7">
         <v>0.85575438106203394</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="9">
+      <c r="A62" s="5">
         <v>-7</v>
       </c>
-      <c r="B62" s="48">
+      <c r="B62" s="41">
         <f t="shared" si="0"/>
         <v>0.19952623149688795</v>
       </c>
-      <c r="C62" s="11">
+      <c r="C62" s="7">
         <v>0.85567334030054398</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="9">
+      <c r="A63" s="5">
         <v>-6</v>
       </c>
-      <c r="B63" s="48">
+      <c r="B63" s="41">
         <f t="shared" si="0"/>
         <v>0.25118864315095801</v>
       </c>
-      <c r="C63" s="11">
+      <c r="C63" s="7">
         <v>0.85340226119018003</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="9">
+      <c r="A64" s="5">
         <v>-5</v>
       </c>
-      <c r="B64" s="48">
+      <c r="B64" s="41">
         <f t="shared" si="0"/>
         <v>0.31622776601683794</v>
       </c>
-      <c r="C64" s="11">
+      <c r="C64" s="7">
         <v>0.84885648322503338</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="9">
+      <c r="A65" s="5">
         <v>-4</v>
       </c>
-      <c r="B65" s="48">
+      <c r="B65" s="41">
         <f t="shared" si="0"/>
         <v>0.3981071705534972</v>
       </c>
-      <c r="C65" s="11">
+      <c r="C65" s="7">
         <v>0.84187150452944892</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="9">
+      <c r="A66" s="5">
         <v>-3</v>
       </c>
-      <c r="B66" s="48">
+      <c r="B66" s="41">
         <f t="shared" si="0"/>
         <v>0.50118723362727224</v>
       </c>
-      <c r="C66" s="11">
+      <c r="C66" s="7">
         <v>0.83220727263234118</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
+      <c r="A67" s="5">
         <v>-2</v>
       </c>
-      <c r="B67" s="48">
+      <c r="B67" s="41">
         <f t="shared" si="0"/>
         <v>0.63095734448019325</v>
       </c>
-      <c r="C67" s="11">
+      <c r="C67" s="7">
         <v>0.81955658418054633</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="9">
+      <c r="A68" s="5">
         <v>-1</v>
       </c>
-      <c r="B68" s="48">
+      <c r="B68" s="41">
         <f t="shared" si="0"/>
         <v>0.79432823472428149</v>
       </c>
-      <c r="C68" s="11">
+      <c r="C68" s="7">
         <v>0.80355987310932908</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
+      <c r="A69" s="5">
         <v>0</v>
       </c>
-      <c r="B69" s="48">
+      <c r="B69" s="41">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C69" s="11">
+      <c r="C69" s="7">
         <v>0.78382911787222842</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="9">
+      <c r="A70" s="5">
         <v>1</v>
       </c>
-      <c r="B70" s="48">
+      <c r="B70" s="41">
         <f t="shared" si="0"/>
         <v>1.2589254117941673</v>
       </c>
-      <c r="C70" s="11">
+      <c r="C70" s="7">
         <v>0.75998350232147471</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="9">
+      <c r="A71" s="5">
         <v>2</v>
       </c>
-      <c r="B71" s="48">
+      <c r="B71" s="41">
         <f t="shared" si="0"/>
         <v>1.5848931924611136</v>
       </c>
-      <c r="C71" s="11">
+      <c r="C71" s="7">
         <v>0.73169838553975253</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="12">
+      <c r="A72" s="8">
         <v>3</v>
       </c>
-      <c r="B72" s="49">
+      <c r="B72" s="42">
         <f t="shared" si="0"/>
         <v>1.9952623149688797</v>
       </c>
-      <c r="C72" s="14">
+      <c r="C72" s="10">
         <v>0.69876661812551233</v>
       </c>
     </row>
@@ -6035,225 +6054,230 @@
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="8"/>
+      <c r="B74" s="56"/>
+      <c r="C74" s="56"/>
+      <c r="D74" s="56"/>
+      <c r="E74" s="56"/>
+      <c r="F74" s="57"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="53" t="s">
+      <c r="A75" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="B75" s="54" t="s">
+      <c r="B75" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="C75" s="54" t="s">
+      <c r="C75" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="D75" s="54" t="s">
+      <c r="D75" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E75" s="54" t="s">
+      <c r="E75" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="F75" s="55" t="s">
+      <c r="F75" s="48" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="53" t="s">
+      <c r="A76" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="B76" s="54" t="s">
+      <c r="B76" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="C76" s="54">
+      <c r="C76" s="47">
         <v>1</v>
       </c>
-      <c r="D76" s="54">
+      <c r="D76" s="47">
         <v>0.31</v>
       </c>
-      <c r="E76" s="56">
+      <c r="E76" s="49">
         <f>D76*C76</f>
         <v>0.31</v>
       </c>
-      <c r="F76" s="55" t="s">
+      <c r="F76" s="48" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="53" t="s">
+      <c r="A77" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B77" s="54" t="s">
+      <c r="B77" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="54">
+      <c r="C77" s="47">
         <v>1</v>
       </c>
-      <c r="D77" s="54">
+      <c r="D77" s="47">
         <v>0.23</v>
       </c>
-      <c r="E77" s="56">
+      <c r="E77" s="49">
         <f>D77*C77</f>
         <v>0.23</v>
       </c>
-      <c r="F77" s="55" t="s">
+      <c r="F77" s="48" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="57" t="s">
+      <c r="A78" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="B78" s="54" t="s">
+      <c r="B78" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="C78" s="54">
+      <c r="C78" s="47">
         <v>1</v>
       </c>
-      <c r="D78" s="54">
+      <c r="D78" s="47">
         <v>0.42</v>
       </c>
-      <c r="E78" s="56">
+      <c r="E78" s="49">
         <f t="shared" ref="E78:E83" si="1">D78*C78</f>
         <v>0.42</v>
       </c>
-      <c r="F78" s="55" t="s">
+      <c r="F78" s="48" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="53" t="s">
+      <c r="A79" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B79" s="54" t="s">
+      <c r="B79" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C79" s="54">
+      <c r="C79" s="47">
         <v>1</v>
       </c>
-      <c r="D79" s="54">
+      <c r="D79" s="47">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E79" s="56">
+      <c r="E79" s="49">
         <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
-      <c r="F79" s="55" t="s">
+      <c r="F79" s="48" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="53" t="s">
+      <c r="A80" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B80" s="54"/>
-      <c r="C80" s="54">
+      <c r="B80" s="47"/>
+      <c r="C80" s="47">
         <v>1</v>
       </c>
-      <c r="D80" s="54">
+      <c r="D80" s="47">
         <v>0.69299999999999995</v>
       </c>
-      <c r="E80" s="56">
+      <c r="E80" s="49">
         <f t="shared" si="1"/>
         <v>0.69299999999999995</v>
       </c>
-      <c r="F80" s="55" t="s">
+      <c r="F80" s="48" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="53" t="s">
+      <c r="A81" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B81" s="54" t="s">
+      <c r="B81" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="C81" s="54">
+      <c r="C81" s="47">
         <v>1</v>
       </c>
-      <c r="D81" s="54">
+      <c r="D81" s="47">
         <v>1.1599999999999999</v>
       </c>
-      <c r="E81" s="56">
+      <c r="E81" s="49">
         <f t="shared" si="1"/>
         <v>1.1599999999999999</v>
       </c>
-      <c r="F81" s="55" t="s">
+      <c r="F81" s="48" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="53" t="s">
+      <c r="A82" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="B82" s="54" t="s">
+      <c r="B82" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="C82" s="54">
+      <c r="C82" s="47">
         <v>1</v>
       </c>
-      <c r="D82" s="54">
+      <c r="D82" s="47">
         <v>0.1</v>
       </c>
-      <c r="E82" s="56">
+      <c r="E82" s="49">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F82" s="55" t="s">
+      <c r="F82" s="48" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="53" t="s">
+      <c r="A83" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B83" s="54"/>
-      <c r="C83" s="54">
+      <c r="B83" s="47"/>
+      <c r="C83" s="47">
         <v>1</v>
       </c>
-      <c r="D83" s="54">
+      <c r="D83" s="47">
         <v>0.16</v>
       </c>
-      <c r="E83" s="60">
+      <c r="E83" s="53">
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-      <c r="F83" s="55" t="s">
+      <c r="F83" s="48" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="53"/>
-      <c r="B84" s="54"/>
-      <c r="C84" s="54"/>
-      <c r="D84" s="54"/>
-      <c r="E84" s="54"/>
-      <c r="F84" s="55"/>
+      <c r="A84" s="46"/>
+      <c r="B84" s="47"/>
+      <c r="C84" s="47"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="48"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="58"/>
-      <c r="B85" s="13" t="s">
+      <c r="A85" s="51"/>
+      <c r="B85" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C85" s="13">
+      <c r="C85" s="9">
         <f>SUM(Table1[Quantity])</f>
         <v>8</v>
       </c>
-      <c r="D85" s="13"/>
-      <c r="E85" s="64">
+      <c r="D85" s="9"/>
+      <c r="E85" s="54">
         <f>SUM(Table1[Price])</f>
         <v>3.363</v>
       </c>
-      <c r="F85" s="59"/>
+      <c r="F85" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A74:F74"/>
@@ -6265,11 +6289,6 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="A34:B34"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
   </mergeCells>
   <conditionalFormatting sqref="G40">
     <cfRule type="colorScale" priority="1">
@@ -6282,26 +6301,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="9" priority="5" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>$G$20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="between">
       <formula>$G$20</formula>
       <formula>1.2*$G$20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>1.2*$G$20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="6" priority="20" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="20" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>$F$28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="21" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="21" operator="between">
       <formula>$F$28</formula>
       <formula>1.2*$F$28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="22" operator="greaterThan">
       <formula>1.2*$F$28</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Stephanie's changes to power tree and conversion calculations
</commit_message>
<xml_diff>
--- a/AOZ1281DI.xlsx
+++ b/AOZ1281DI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred\Downloads\SBC5-Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\SBC5-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0D6E96-90B7-413D-9E74-F2C6D12CEC73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42193EC4-010F-4369-826C-EE03C1A79576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{D55AB5B1-4BC1-429F-82B8-F59F2B41C856}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19635" windowHeight="13875" activeTab="1" xr2:uid="{D55AB5B1-4BC1-429F-82B8-F59F2B41C856}"/>
   </bookViews>
   <sheets>
     <sheet name="5V" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="97">
   <si>
     <t>R1</t>
   </si>
@@ -313,9 +313,6 @@
     <t>49.9k</t>
   </si>
   <si>
-    <t>ERA-6AEB4992V</t>
-  </si>
-  <si>
     <t>ERJ-PB3B1372V</t>
   </si>
   <si>
@@ -363,6 +360,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>ERA-3AEB4992V</t>
+  </si>
+  <si>
+    <t>ERA-3AEB9531V</t>
+  </si>
+  <si>
+    <t>9.53k</t>
   </si>
 </sst>
 </file>
@@ -378,7 +384,7 @@
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +414,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -427,7 +439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -716,19 +728,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -737,7 +736,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -775,9 +774,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -844,9 +840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -1195,70 +1189,70 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>0.69059042379965763</c:v>
+                  <c:v>0.68796144368040457</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.72798037471181143</c:v>
+                  <c:v>0.72565841564890254</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76060363662403097</c:v>
+                  <c:v>0.75858913479286583</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.78855388622133216</c:v>
+                  <c:v>0.78683314060841636</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81209798050687554</c:v>
+                  <c:v>0.81064772924535222</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.83160747875367458</c:v>
+                  <c:v>0.83039908659056849</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.84749971890299669</c:v>
+                  <c:v>0.8465025459682527</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.86019232949422586</c:v>
+                  <c:v>0.85937615782215837</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.87007125498392679</c:v>
+                  <c:v>0.86940784649076053</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.87747023089874654</c:v>
+                  <c:v>0.87693418491977115</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.8826588454799541</c:v>
+                  <c:v>0.88222794563366036</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.88583637781754987</c:v>
+                  <c:v>0.88549159897513474</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.88712908675677771</c:v>
+                  <c:v>0.88685439742453465</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.88658926267951899</c:v>
+                  <c:v>0.88637132073878222</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.88419500431857101</c:v>
+                  <c:v>0.88402281183909759</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.87985030029745082</c:v>
+                  <c:v>0.87971485829539897</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.87338559069235189</c:v>
+                  <c:v>0.87327957699602976</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.86455958928421106</c:v>
+                  <c:v>0.86447707083421754</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.85306378530717675</c:v>
+                  <c:v>0.85299996877927298</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.83853169694160123</c:v>
+                  <c:v>0.8384827172270144</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.82055552106432095</c:v>
+                  <c:v>0.82051826483691459</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.79871309698574922</c:v>
+                  <c:v>0.79868505756637986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3671,47 +3665,47 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="57"/>
-    </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="27" t="s">
         <v>27</v>
       </c>
@@ -3724,15 +3718,15 @@
       <c r="D2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="65"/>
+      <c r="F2" s="64"/>
       <c r="G2" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -3755,7 +3749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="15">
         <v>0.8</v>
       </c>
@@ -3779,26 +3773,26 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+    <row r="5" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
-    </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="56"/>
+    </row>
+    <row r="7" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="30" t="s">
@@ -3834,40 +3828,40 @@
       <c r="L7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23">
         <v>1E-3</v>
       </c>
       <c r="B8" s="16">
-        <v>147000</v>
+        <v>49900</v>
       </c>
       <c r="C8" s="24">
         <f>A4*B8/(B4-A4)</f>
-        <v>28000</v>
+        <v>9504.7619047619046</v>
       </c>
       <c r="D8" s="11">
         <f>B8*(1-A8)</f>
-        <v>146853</v>
+        <v>49850.1</v>
       </c>
       <c r="E8" s="11">
         <f>B8*(1+A8)</f>
-        <v>147146.99999999997</v>
+        <v>49949.899999999994</v>
       </c>
       <c r="F8" s="20">
         <f>C8*(1-A8)</f>
-        <v>27972</v>
+        <v>9495.2571428571428</v>
       </c>
       <c r="G8" s="20">
         <f>C8*(1+A8)</f>
-        <v>28027.999999999996</v>
+        <v>9514.2666666666646</v>
       </c>
       <c r="H8" s="21">
         <f>A4*(1+D8/G8)</f>
-        <v>4.9916083916083922</v>
+        <v>4.9916083916083931</v>
       </c>
       <c r="I8" s="21">
         <f>A4*(1+B8/C8)</f>
@@ -3875,41 +3869,41 @@
       </c>
       <c r="J8" s="21">
         <f>A4*(1+E8/F8)</f>
-        <v>5.0084084084084077</v>
+        <v>5.0084084084084086</v>
       </c>
       <c r="K8" s="21">
         <f>ABS(MAX(J8, H8)-B4)</f>
-        <v>8.4084084084077304E-3</v>
+        <v>8.4084084084086186E-3</v>
       </c>
       <c r="L8" s="25">
         <f>K8/B4</f>
-        <v>1.681681681681546E-3</v>
-      </c>
-      <c r="M8" s="36">
+        <v>1.6816816816817236E-3</v>
+      </c>
+      <c r="M8" s="35">
         <f>J8^2/(E8+F8)</f>
-        <v>1.4324062372110419E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+        <v>4.2197137649303254E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="57"/>
-    </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="56"/>
+    </row>
+    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="30" t="s">
@@ -3945,83 +3939,83 @@
       <c r="L11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="33" t="s">
+      <c r="M11" s="32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="23">
         <v>1E-3</v>
       </c>
       <c r="B12" s="16">
         <f>B8</f>
-        <v>147000</v>
+        <v>49900</v>
       </c>
       <c r="C12" s="19">
-        <v>28000</v>
+        <v>9530</v>
       </c>
       <c r="D12" s="11">
         <f>B12*(1-A12)</f>
-        <v>146853</v>
+        <v>49850.1</v>
       </c>
       <c r="E12" s="11">
         <f>B12*(1+A12)</f>
-        <v>147146.99999999997</v>
+        <v>49949.899999999994</v>
       </c>
       <c r="F12" s="20">
         <f>C12*(1-A12)</f>
-        <v>27972</v>
+        <v>9520.4699999999993</v>
       </c>
       <c r="G12" s="20">
         <f>C12*(1+A12)</f>
-        <v>28027.999999999996</v>
+        <v>9539.5299999999988</v>
       </c>
       <c r="H12" s="21">
         <f>A4*(1+D12/G12)</f>
-        <v>4.9916083916083922</v>
+        <v>4.9805078447261035</v>
       </c>
       <c r="I12" s="21">
         <f>A4*(1+B12/C12)</f>
-        <v>5</v>
+        <v>4.9888772298006296</v>
       </c>
       <c r="J12" s="21">
         <f>A4*(1+E12/F12)</f>
-        <v>5.0084084084084077</v>
+        <v>4.9972633704008311</v>
       </c>
       <c r="K12" s="21">
         <f>ABS(MAX(J12, H12)-B4)</f>
-        <v>8.4084084084077304E-3</v>
+        <v>2.7366295991688716E-3</v>
       </c>
       <c r="L12" s="22">
         <f>K12/B4</f>
-        <v>1.681681681681546E-3</v>
-      </c>
-      <c r="M12" s="36">
+        <v>5.4732591983377434E-4</v>
+      </c>
+      <c r="M12" s="35">
         <f>J12*J12/(E12+F12)</f>
-        <v>1.4324062372110419E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+        <v>4.1991736713845696E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="57"/>
-      <c r="E14" s="55" t="s">
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="E14" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
+    </row>
+    <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="32" t="s">
         <v>44</v>
       </c>
       <c r="E15" s="27" t="s">
@@ -4030,11 +4024,11 @@
       <c r="F15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="32" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="15">
         <v>0.01</v>
       </c>
@@ -4042,7 +4036,7 @@
         <f>(D4/(E4*A16))*(1-B4/C4)*(B4/C4)</f>
         <v>2.0254629629629626E-5</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="36">
         <f>D4*SQRT((B4/C4)*(1-B4/C4))</f>
         <v>0.49300664859163462</v>
       </c>
@@ -4054,32 +4048,32 @@
         <f>(D4/(E4*E16))*(1-B4/C4)*(B4/C4)</f>
         <v>1.8413299663299664E-3</v>
       </c>
-      <c r="G16" s="37">
+      <c r="G16" s="36">
         <f>D4*SQRT((B4/C4)*(1-B4/C4))</f>
         <v>0.49300664859163462</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
+    <row r="17" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
-      <c r="E18" s="55" t="s">
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="E18" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F18" s="55"/>
+      <c r="G18" s="56"/>
+    </row>
+    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="27" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>45</v>
       </c>
       <c r="E19" s="27" t="s">
@@ -4088,15 +4082,15 @@
       <c r="F19" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="15">
         <v>0.01</v>
       </c>
-      <c r="B20" s="35">
+      <c r="B20" s="34">
         <f>(B4/(E4*A20))*(1-B4/C4)</f>
         <v>2.4305555555555555E-4</v>
       </c>
@@ -4111,28 +4105,28 @@
         <f>(B4/(E4*E20))*(1-B4/C4)</f>
         <v>1.1047979797979796E-2</v>
       </c>
-      <c r="G20" s="37">
+      <c r="G20" s="36">
         <f>D4+F20/2</f>
         <v>1.0055239898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
+    <row r="21" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="63"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="62"/>
+    </row>
+    <row r="23" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>49</v>
@@ -4143,15 +4137,15 @@
       <c r="E23" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="15">
         <v>0.01</v>
       </c>
-      <c r="B24" s="39">
+      <c r="B24" s="38">
         <v>0.125</v>
       </c>
       <c r="C24" s="21">
@@ -4166,28 +4160,28 @@
         <f>A20/SQRT(12)</f>
         <v>2.886751345948129E-3</v>
       </c>
-      <c r="F24" s="37">
+      <c r="F24" s="36">
         <f>A24+B4</f>
         <v>5.01</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="61" t="s">
+    <row r="25" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="63"/>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="62"/>
+    </row>
+    <row r="27" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="27" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>49</v>
@@ -4198,18 +4192,18 @@
       <c r="E27" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="38">
+    <row r="28" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A28" s="37">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="B28" s="39">
+      <c r="B28" s="38">
         <v>0.125</v>
       </c>
-      <c r="C28" s="40">
+      <c r="C28" s="39">
         <f>B28/(2*PI()*E4*A28)</f>
         <v>1.6578639905405763E-2</v>
       </c>
@@ -4221,23 +4215,23 @@
         <f>F20/SQRT(12)</f>
         <v>3.1892770551825915E-3</v>
       </c>
-      <c r="F28" s="37">
+      <c r="F28" s="36">
         <f>D28+J12</f>
-        <v>5.0097424001161173</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="55" t="s">
+        <v>4.9985973621085407</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="56"/>
+    </row>
+    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="27" t="s">
         <v>53</v>
       </c>
@@ -4253,11 +4247,11 @@
       <c r="E31" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="15">
         <v>0.5</v>
       </c>
@@ -4279,43 +4273,43 @@
         <v>32.800000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="55" t="s">
+    <row r="33" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="57"/>
-    </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="56"/>
+    </row>
+    <row r="35" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="15">
         <v>0.38</v>
       </c>
-      <c r="B36" s="37">
+      <c r="B36" s="36">
         <f>1.1*G20^2*A36</f>
         <v>0.42263081060167651</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="55" t="s">
+    <row r="37" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="57"/>
-    </row>
-    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="56"/>
+    </row>
+    <row r="39" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" s="27" t="s">
         <v>61</v>
       </c>
@@ -4334,11 +4328,11 @@
       <c r="F39" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G39" s="33" t="s">
+      <c r="G39" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A40" s="14">
         <f>0.38+(C4-3.3)*(0.24-0.38)/(12-3.3)</f>
         <v>0.24</v>
@@ -4366,16 +4360,16 @@
         <v>14.336236124263467</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="55" t="s">
+    <row r="41" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A42" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="57"/>
-    </row>
-    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="56"/>
+    </row>
+    <row r="43" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="27" t="s">
         <v>66</v>
       </c>
@@ -4385,43 +4379,43 @@
       <c r="C43" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="44">
+    <row r="44" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A44" s="43">
         <f>E40+B36+E32+M12</f>
-        <v>1.0934328898483698</v>
+        <v>1.0937095665917871</v>
       </c>
       <c r="B44" s="21">
         <f>B4*D4+A44</f>
-        <v>6.0934328898483701</v>
-      </c>
-      <c r="C44" s="43">
+        <v>6.0937095665917873</v>
+      </c>
+      <c r="C44" s="42">
         <f>B4*D4/B44</f>
-        <v>0.82055552106432095</v>
-      </c>
-      <c r="D44" s="37">
+        <v>0.82051826483691459</v>
+      </c>
+      <c r="D44" s="36">
         <f>B44/C4</f>
-        <v>0.50778607415403088</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="55" t="s">
+        <v>0.50780913054931565</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A46" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="56"/>
-      <c r="C46" s="57"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="56"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="34" t="s">
+    <row r="47" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A47" s="33" t="s">
         <v>12</v>
       </c>
       <c r="B47" s="30" t="s">
@@ -4431,500 +4425,500 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="5"/>
       <c r="B48" s="4"/>
       <c r="C48" s="7">
         <f>C44</f>
-        <v>0.82055552106432095</v>
+        <v>0.82051826483691459</v>
       </c>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="5">
         <v>-20</v>
       </c>
-      <c r="B49" s="41">
+      <c r="B49" s="40">
         <f>10^(A49/10)</f>
         <v>0.01</v>
       </c>
       <c r="C49" s="7">
         <f t="dataTable" ref="C49:C70" dt2D="0" dtr="0" r1="D4"/>
-        <v>0.69059042379965763</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.68796144368040457</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="5">
         <v>-19</v>
       </c>
-      <c r="B50" s="41">
+      <c r="B50" s="40">
         <f t="shared" ref="B50:B70" si="0">10^(A50/10)</f>
         <v>1.2589254117941664E-2</v>
       </c>
       <c r="C50" s="7">
-        <v>0.72798037471181143</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.72565841564890254</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="5">
         <v>-18</v>
       </c>
-      <c r="B51" s="41">
+      <c r="B51" s="40">
         <f t="shared" si="0"/>
         <v>1.5848931924611124E-2</v>
       </c>
       <c r="C51" s="7">
-        <v>0.76060363662403097</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.75858913479286583</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" s="5">
         <v>-17</v>
       </c>
-      <c r="B52" s="41">
+      <c r="B52" s="40">
         <f t="shared" si="0"/>
         <v>1.9952623149688792E-2</v>
       </c>
       <c r="C52" s="7">
-        <v>0.78855388622133216</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.78683314060841636</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" s="5">
         <v>-16</v>
       </c>
-      <c r="B53" s="41">
+      <c r="B53" s="40">
         <f t="shared" si="0"/>
         <v>2.511886431509578E-2</v>
       </c>
       <c r="C53" s="7">
-        <v>0.81209798050687554</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.81064772924535222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" s="5">
         <v>-15</v>
       </c>
-      <c r="B54" s="41">
+      <c r="B54" s="40">
         <f t="shared" si="0"/>
         <v>3.1622776601683784E-2</v>
       </c>
       <c r="C54" s="7">
-        <v>0.83160747875367458</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.83039908659056849</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" s="5">
         <v>-14</v>
       </c>
-      <c r="B55" s="41">
+      <c r="B55" s="40">
         <f t="shared" si="0"/>
         <v>3.9810717055349727E-2</v>
       </c>
       <c r="C55" s="7">
-        <v>0.84749971890299669</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.8465025459682527</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" s="5">
         <v>-13</v>
       </c>
-      <c r="B56" s="41">
+      <c r="B56" s="40">
         <f t="shared" si="0"/>
         <v>5.0118723362727206E-2</v>
       </c>
       <c r="C56" s="7">
-        <v>0.86019232949422586</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.85937615782215837</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" s="5">
         <v>-12</v>
       </c>
-      <c r="B57" s="41">
+      <c r="B57" s="40">
         <f t="shared" si="0"/>
         <v>6.3095734448019317E-2</v>
       </c>
       <c r="C57" s="7">
-        <v>0.87007125498392679</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.86940784649076053</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" s="5">
         <v>-11</v>
       </c>
-      <c r="B58" s="41">
+      <c r="B58" s="40">
         <f t="shared" si="0"/>
         <v>7.9432823472428096E-2</v>
       </c>
       <c r="C58" s="7">
-        <v>0.87747023089874654</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.87693418491977115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" s="5">
         <v>-10</v>
       </c>
-      <c r="B59" s="41">
+      <c r="B59" s="40">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="C59" s="7">
-        <v>0.8826588454799541</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.88222794563366036</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" s="5">
         <v>-9</v>
       </c>
-      <c r="B60" s="41">
+      <c r="B60" s="40">
         <f t="shared" si="0"/>
         <v>0.12589254117941667</v>
       </c>
       <c r="C60" s="7">
-        <v>0.88583637781754987</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.88549159897513474</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" s="5">
         <v>-8</v>
       </c>
-      <c r="B61" s="41">
+      <c r="B61" s="40">
         <f t="shared" si="0"/>
         <v>0.15848931924611132</v>
       </c>
       <c r="C61" s="7">
-        <v>0.88712908675677771</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.88685439742453465</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" s="5">
         <v>-7</v>
       </c>
-      <c r="B62" s="41">
+      <c r="B62" s="40">
         <f t="shared" si="0"/>
         <v>0.19952623149688795</v>
       </c>
       <c r="C62" s="7">
-        <v>0.88658926267951899</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.88637132073878222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" s="5">
         <v>-6</v>
       </c>
-      <c r="B63" s="41">
+      <c r="B63" s="40">
         <f t="shared" si="0"/>
         <v>0.25118864315095801</v>
       </c>
       <c r="C63" s="7">
-        <v>0.88419500431857101</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.88402281183909759</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" s="5">
         <v>-5</v>
       </c>
-      <c r="B64" s="41">
+      <c r="B64" s="40">
         <f t="shared" si="0"/>
         <v>0.31622776601683794</v>
       </c>
       <c r="C64" s="7">
-        <v>0.87985030029745082</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.87971485829539897</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="5">
         <v>-4</v>
       </c>
-      <c r="B65" s="41">
+      <c r="B65" s="40">
         <f t="shared" si="0"/>
         <v>0.3981071705534972</v>
       </c>
       <c r="C65" s="7">
-        <v>0.87338559069235189</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.87327957699602976</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="5">
         <v>-3</v>
       </c>
-      <c r="B66" s="41">
+      <c r="B66" s="40">
         <f t="shared" si="0"/>
         <v>0.50118723362727224</v>
       </c>
       <c r="C66" s="7">
-        <v>0.86455958928421106</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.86447707083421754</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="5">
         <v>-2</v>
       </c>
-      <c r="B67" s="41">
+      <c r="B67" s="40">
         <f t="shared" si="0"/>
         <v>0.63095734448019325</v>
       </c>
       <c r="C67" s="7">
-        <v>0.85306378530717675</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.85299996877927298</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="5">
         <v>-1</v>
       </c>
-      <c r="B68" s="41">
+      <c r="B68" s="40">
         <f t="shared" si="0"/>
         <v>0.79432823472428149</v>
       </c>
       <c r="C68" s="7">
-        <v>0.83853169694160123</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.8384827172270144</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="5">
         <v>0</v>
       </c>
-      <c r="B69" s="41">
+      <c r="B69" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C69" s="7">
-        <v>0.82055552106432095</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.82051826483691459</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A70" s="8">
         <v>1</v>
       </c>
-      <c r="B70" s="42">
+      <c r="B70" s="41">
         <f t="shared" si="0"/>
         <v>1.2589254117941673</v>
       </c>
       <c r="C70" s="10">
-        <v>0.79871309698574922</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.79868505756637986</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="58" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="59"/>
-      <c r="C72" s="59"/>
-      <c r="D72" s="59"/>
-      <c r="E72" s="59"/>
-      <c r="F72" s="60"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="46" t="s">
+      <c r="B72" s="58"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="58"/>
+      <c r="E72" s="58"/>
+      <c r="F72" s="59"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B73" s="47" t="s">
+      <c r="B73" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="C73" s="47" t="s">
+      <c r="C73" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="D73" s="47" t="s">
+      <c r="D73" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="E73" s="47" t="s">
+      <c r="E73" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="F73" s="48" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B74" s="47" t="s">
+      <c r="F73" s="47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C74" s="47">
+      <c r="C74" s="46">
         <v>1</v>
       </c>
-      <c r="D74" s="47">
+      <c r="D74" s="46">
         <v>0.31</v>
       </c>
-      <c r="E74" s="49">
+      <c r="E74" s="48">
         <f>D74*C74</f>
         <v>0.31</v>
       </c>
-      <c r="F74" s="48" t="s">
+      <c r="F74" s="47" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="B75" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="C75" s="47">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B75" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="C75" s="46">
         <v>1</v>
       </c>
-      <c r="D75" s="47">
-        <v>0.23</v>
-      </c>
-      <c r="E75" s="49">
+      <c r="D75" s="46">
+        <v>0.31</v>
+      </c>
+      <c r="E75" s="48">
         <f>D75*C75</f>
-        <v>0.23</v>
-      </c>
-      <c r="F75" s="48" t="s">
+        <v>0.31</v>
+      </c>
+      <c r="F75" s="47" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="B76" s="47" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C76" s="47">
+      <c r="B76" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" s="46">
         <v>1</v>
       </c>
-      <c r="D76" s="47">
+      <c r="D76" s="46">
         <v>0.42</v>
       </c>
-      <c r="E76" s="49">
+      <c r="E76" s="48">
         <f t="shared" ref="E76:E81" si="1">D76*C76</f>
         <v>0.42</v>
       </c>
-      <c r="F76" s="48" t="s">
+      <c r="F76" s="47" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="46" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B77" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="C77" s="47">
+      <c r="C77" s="46">
         <v>1</v>
       </c>
-      <c r="D77" s="47">
+      <c r="D77" s="46">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E77" s="49">
+      <c r="E77" s="48">
         <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
-      <c r="F77" s="48" t="s">
+      <c r="F77" s="47" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="B78" s="47"/>
-      <c r="C78" s="47">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B78" s="46"/>
+      <c r="C78" s="46">
         <v>1</v>
       </c>
-      <c r="D78" s="47">
+      <c r="D78" s="46">
         <v>0.69299999999999995</v>
       </c>
-      <c r="E78" s="49">
+      <c r="E78" s="48">
         <f t="shared" si="1"/>
         <v>0.69299999999999995</v>
       </c>
-      <c r="F78" s="48" t="s">
+      <c r="F78" s="47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B79" s="46" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="B79" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="C79" s="47">
+      <c r="C79" s="46">
         <v>1</v>
       </c>
-      <c r="D79" s="47">
+      <c r="D79" s="46">
         <v>1.1599999999999999</v>
       </c>
-      <c r="E79" s="49">
+      <c r="E79" s="48">
         <f t="shared" si="1"/>
         <v>1.1599999999999999</v>
       </c>
-      <c r="F79" s="48" t="s">
+      <c r="F79" s="47" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B80" s="47" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C80" s="47">
+      <c r="B80" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C80" s="46">
         <v>1</v>
       </c>
-      <c r="D80" s="47">
+      <c r="D80" s="46">
         <v>0.1</v>
       </c>
-      <c r="E80" s="49">
+      <c r="E80" s="48">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F80" s="48" t="s">
+      <c r="F80" s="47" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="B81" s="47"/>
-      <c r="C81" s="47">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A81" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B81" s="46"/>
+      <c r="C81" s="46">
         <v>1</v>
       </c>
-      <c r="D81" s="47">
+      <c r="D81" s="46">
         <v>0.16</v>
       </c>
-      <c r="E81" s="53">
+      <c r="E81" s="52">
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-      <c r="F81" s="48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="46"/>
-      <c r="B82" s="47"/>
-      <c r="C82" s="47"/>
-      <c r="D82" s="47"/>
-      <c r="E82" s="47"/>
-      <c r="F82" s="48"/>
-    </row>
-    <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="51"/>
+      <c r="F81" s="47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A82" s="45"/>
+      <c r="B82" s="46"/>
+      <c r="C82" s="46"/>
+      <c r="D82" s="46"/>
+      <c r="E82" s="46"/>
+      <c r="F82" s="47"/>
+    </row>
+    <row r="83" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A83" s="50"/>
       <c r="B83" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C83" s="9">
         <f>SUM(Table2[Quantity])</f>
         <v>8</v>
       </c>
       <c r="D83" s="9"/>
-      <c r="E83" s="54">
+      <c r="E83" s="53">
         <f>SUM(Table2[Price])</f>
-        <v>3.363</v>
-      </c>
-      <c r="F83" s="52"/>
+        <v>3.4430000000000001</v>
+      </c>
+      <c r="F83" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -4992,47 +4986,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5CAF6-20E4-4B67-AE88-D57C6FEB2845}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="57"/>
-    </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="27" t="s">
         <v>27</v>
       </c>
@@ -5045,15 +5039,15 @@
       <c r="D2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="65"/>
+      <c r="F2" s="64"/>
       <c r="G2" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -5076,7 +5070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="15">
         <v>0.8</v>
       </c>
@@ -5100,26 +5094,26 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+    <row r="5" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
-    </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="56"/>
+    </row>
+    <row r="7" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="30" t="s">
@@ -5155,11 +5149,11 @@
       <c r="L7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="23">
         <v>1E-3</v>
       </c>
@@ -5206,31 +5200,31 @@
         <f>K8/B4</f>
         <v>1.56913670427205E-3</v>
       </c>
-      <c r="M8" s="36">
+      <c r="M8" s="35">
         <f>J8^2/(E8+F8)</f>
         <v>2.1558305473483194E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+    <row r="9" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="57"/>
-    </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="32" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="56"/>
+    </row>
+    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="30" t="s">
@@ -5266,11 +5260,11 @@
       <c r="L11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="33" t="s">
+      <c r="M11" s="32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="23">
         <v>1E-3</v>
       </c>
@@ -5317,45 +5311,45 @@
         <f>K12/B4</f>
         <v>5.3249145772325699E-3</v>
       </c>
-      <c r="M12" s="36">
+      <c r="M12" s="35">
         <f>J12*J12/(E12+F12)</f>
         <v>2.1742631296614928E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+    <row r="13" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="57"/>
-      <c r="E14" s="55" t="s">
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="E14" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
+    </row>
+    <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="66" t="s">
+      <c r="E15" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="32" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="15">
         <v>0.01</v>
       </c>
@@ -5363,7 +5357,7 @@
         <f>(D4/(E4*A16))*(1-B4/C4)*(B4/C4)</f>
         <v>2.6569126157407413E-5</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="36">
         <f>D4*SQRT((B4/C4)*(1-B4/C4))</f>
         <v>0.69039852495778764</v>
       </c>
@@ -5375,32 +5369,32 @@
         <f>(D4/(E4*E16))*(1-B4/C4)*(B4/C4)</f>
         <v>2.4153751052188553E-3</v>
       </c>
-      <c r="G16" s="37">
+      <c r="G16" s="36">
         <f>D4*SQRT((B4/C4)*(1-B4/C4))</f>
         <v>0.69039852495778764</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
+    <row r="17" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
-      <c r="E18" s="55" t="s">
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="E18" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F18" s="55"/>
+      <c r="G18" s="56"/>
+    </row>
+    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="27" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>45</v>
       </c>
       <c r="E19" s="27" t="s">
@@ -5409,15 +5403,15 @@
       <c r="F19" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="15">
         <v>0.01</v>
       </c>
-      <c r="B20" s="35">
+      <c r="B20" s="34">
         <f>(B4/(E4*A20))*(1-B4/C4)</f>
         <v>2.1326388888888889E-4</v>
       </c>
@@ -5432,28 +5426,28 @@
         <f>(B4/(E4*E20))*(1-B4/C4)</f>
         <v>9.6938131313131313E-3</v>
       </c>
-      <c r="G20" s="37">
+      <c r="G20" s="36">
         <f>D4+F20/2</f>
         <v>1.4998469065656568</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
+    <row r="21" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="63"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="61"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="62"/>
+    </row>
+    <row r="23" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>49</v>
@@ -5464,15 +5458,15 @@
       <c r="E23" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="15">
         <v>0.01</v>
       </c>
-      <c r="B24" s="45">
+      <c r="B24" s="44">
         <v>0.125</v>
       </c>
       <c r="C24" s="21">
@@ -5492,23 +5486,23 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="61" t="s">
+    <row r="25" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="63"/>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="62"/>
+    </row>
+    <row r="27" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="27" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>49</v>
@@ -5519,18 +5513,18 @@
       <c r="E27" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="38">
+    <row r="28" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A28" s="37">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="B28" s="45">
+      <c r="B28" s="44">
         <v>0.125</v>
       </c>
-      <c r="C28" s="40">
+      <c r="C28" s="39">
         <f>B28/(2*PI()*E4*A28)</f>
         <v>1.6578639905405763E-2</v>
       </c>
@@ -5542,23 +5536,23 @@
         <f>F20/SQRT(12)</f>
         <v>2.7983628104187828E-3</v>
       </c>
-      <c r="F28" s="37">
+      <c r="F28" s="36">
         <f>D28+J12</f>
         <v>3.7208726663741536</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="55" t="s">
+    <row r="29" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="56"/>
+    </row>
+    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="27" t="s">
         <v>53</v>
       </c>
@@ -5574,11 +5568,11 @@
       <c r="E31" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="15">
         <v>0.5</v>
       </c>
@@ -5600,43 +5594,43 @@
         <v>49.036000000000008</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="55" t="s">
+    <row r="33" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="57"/>
-    </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="56"/>
+    </row>
+    <row r="35" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A35" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="15">
         <v>0.315</v>
       </c>
-      <c r="B36" s="37">
+      <c r="B36" s="36">
         <f>1.1*G20^2*A36</f>
         <v>0.77946586749612856</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="55" t="s">
+    <row r="37" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="57"/>
-    </row>
-    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="55"/>
+      <c r="G38" s="56"/>
+    </row>
+    <row r="39" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" s="27" t="s">
         <v>61</v>
       </c>
@@ -5655,11 +5649,11 @@
       <c r="F39" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="G39" s="33" t="s">
+      <c r="G39" s="32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A40" s="14">
         <f>0.38+(C4-3.3)*(0.24-0.38)/(12-3.3)</f>
         <v>0.24</v>
@@ -5687,16 +5681,16 @@
         <v>30.683937809376324</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="55" t="s">
+    <row r="41" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A42" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="57"/>
-    </row>
-    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="56"/>
+    </row>
+    <row r="43" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="27" t="s">
         <v>66</v>
       </c>
@@ -5706,12 +5700,12 @@
       <c r="C43" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="44">
+    <row r="44" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A44" s="43">
         <f>E40+B36+E32+M12</f>
         <v>1.9505230721613918</v>
       </c>
@@ -5723,26 +5717,26 @@
         <f>B4*D4/B44</f>
         <v>0.73930539195758871</v>
       </c>
-      <c r="D44" s="37">
+      <c r="D44" s="36">
         <f>B44/C4</f>
         <v>0.62350192268011606</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="55" t="s">
+    <row r="45" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A46" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="56"/>
-      <c r="C46" s="57"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="56"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="34" t="s">
+    <row r="47" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A47" s="33" t="s">
         <v>12</v>
       </c>
       <c r="B47" s="30" t="s">
@@ -5752,7 +5746,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="5"/>
       <c r="B48" s="4"/>
       <c r="C48" s="7">
@@ -5761,11 +5755,11 @@
       </c>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="5">
         <v>-20</v>
       </c>
-      <c r="B49" s="41">
+      <c r="B49" s="40">
         <f>10^(A49/10)</f>
         <v>0.01</v>
       </c>
@@ -5774,11 +5768,11 @@
         <v>0.62240619702935862</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="5">
         <v>-19</v>
       </c>
-      <c r="B50" s="41">
+      <c r="B50" s="40">
         <f t="shared" ref="B50:B72" si="0">10^(A50/10)</f>
         <v>1.2589254117941664E-2</v>
       </c>
@@ -5786,11 +5780,11 @@
         <v>0.66412682063428197</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" s="5">
         <v>-18</v>
       </c>
-      <c r="B51" s="41">
+      <c r="B51" s="40">
         <f t="shared" si="0"/>
         <v>1.5848931924611124E-2</v>
       </c>
@@ -5798,11 +5792,11 @@
         <v>0.70138296650231557</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" s="5">
         <v>-17</v>
       </c>
-      <c r="B52" s="41">
+      <c r="B52" s="40">
         <f t="shared" si="0"/>
         <v>1.9952623149688792E-2</v>
       </c>
@@ -5810,11 +5804,11 @@
         <v>0.73396499657999337</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" s="5">
         <v>-16</v>
       </c>
-      <c r="B53" s="41">
+      <c r="B53" s="40">
         <f t="shared" si="0"/>
         <v>2.511886431509578E-2</v>
       </c>
@@ -5822,11 +5816,11 @@
         <v>0.76191025850561611</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" s="5">
         <v>-15</v>
       </c>
-      <c r="B54" s="41">
+      <c r="B54" s="40">
         <f t="shared" si="0"/>
         <v>3.1622776601683784E-2</v>
       </c>
@@ -5834,11 +5828,11 @@
         <v>0.78543698075365709</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" s="5">
         <v>-14</v>
       </c>
-      <c r="B55" s="41">
+      <c r="B55" s="40">
         <f t="shared" si="0"/>
         <v>3.9810717055349727E-2</v>
       </c>
@@ -5846,11 +5840,11 @@
         <v>0.80487597113032094</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" s="5">
         <v>-13</v>
       </c>
-      <c r="B56" s="41">
+      <c r="B56" s="40">
         <f t="shared" si="0"/>
         <v>5.0118723362727206E-2</v>
       </c>
@@ -5858,11 +5852,11 @@
         <v>0.82061010469092444</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" s="5">
         <v>-12</v>
       </c>
-      <c r="B57" s="41">
+      <c r="B57" s="40">
         <f t="shared" si="0"/>
         <v>6.3095734448019317E-2</v>
       </c>
@@ -5870,11 +5864,11 @@
         <v>0.83302635349491971</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" s="5">
         <v>-11</v>
       </c>
-      <c r="B58" s="41">
+      <c r="B58" s="40">
         <f t="shared" si="0"/>
         <v>7.9432823472428096E-2</v>
       </c>
@@ -5882,11 +5876,11 @@
         <v>0.8424810761986421</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" s="5">
         <v>-10</v>
       </c>
-      <c r="B59" s="41">
+      <c r="B59" s="40">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -5894,11 +5888,11 @@
         <v>0.84927688713019533</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" s="5">
         <v>-9</v>
       </c>
-      <c r="B60" s="41">
+      <c r="B60" s="40">
         <f t="shared" si="0"/>
         <v>0.12589254117941667</v>
       </c>
@@ -5906,11 +5900,11 @@
         <v>0.85364843514519362</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" s="5">
         <v>-8</v>
       </c>
-      <c r="B61" s="41">
+      <c r="B61" s="40">
         <f t="shared" si="0"/>
         <v>0.15848931924611132</v>
       </c>
@@ -5918,11 +5912,11 @@
         <v>0.85575438106203394</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" s="5">
         <v>-7</v>
       </c>
-      <c r="B62" s="41">
+      <c r="B62" s="40">
         <f t="shared" si="0"/>
         <v>0.19952623149688795</v>
       </c>
@@ -5930,11 +5924,11 @@
         <v>0.85567334030054398</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" s="5">
         <v>-6</v>
       </c>
-      <c r="B63" s="41">
+      <c r="B63" s="40">
         <f t="shared" si="0"/>
         <v>0.25118864315095801</v>
       </c>
@@ -5942,11 +5936,11 @@
         <v>0.85340226119018003</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" s="5">
         <v>-5</v>
       </c>
-      <c r="B64" s="41">
+      <c r="B64" s="40">
         <f t="shared" si="0"/>
         <v>0.31622776601683794</v>
       </c>
@@ -5954,11 +5948,11 @@
         <v>0.84885648322503338</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="5">
         <v>-4</v>
       </c>
-      <c r="B65" s="41">
+      <c r="B65" s="40">
         <f t="shared" si="0"/>
         <v>0.3981071705534972</v>
       </c>
@@ -5966,11 +5960,11 @@
         <v>0.84187150452944892</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="5">
         <v>-3</v>
       </c>
-      <c r="B66" s="41">
+      <c r="B66" s="40">
         <f t="shared" si="0"/>
         <v>0.50118723362727224</v>
       </c>
@@ -5978,11 +5972,11 @@
         <v>0.83220727263234118</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="5">
         <v>-2</v>
       </c>
-      <c r="B67" s="41">
+      <c r="B67" s="40">
         <f t="shared" si="0"/>
         <v>0.63095734448019325</v>
       </c>
@@ -5990,11 +5984,11 @@
         <v>0.81955658418054633</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="5">
         <v>-1</v>
       </c>
-      <c r="B68" s="41">
+      <c r="B68" s="40">
         <f t="shared" si="0"/>
         <v>0.79432823472428149</v>
       </c>
@@ -6002,11 +5996,11 @@
         <v>0.80355987310932908</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="5">
         <v>0</v>
       </c>
-      <c r="B69" s="41">
+      <c r="B69" s="40">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -6014,11 +6008,11 @@
         <v>0.78382911787222842</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="5">
         <v>1</v>
       </c>
-      <c r="B70" s="41">
+      <c r="B70" s="40">
         <f t="shared" si="0"/>
         <v>1.2589254117941673</v>
       </c>
@@ -6026,11 +6020,11 @@
         <v>0.75998350232147471</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="5">
         <v>2</v>
       </c>
-      <c r="B71" s="41">
+      <c r="B71" s="40">
         <f t="shared" si="0"/>
         <v>1.5848931924611136</v>
       </c>
@@ -6038,11 +6032,11 @@
         <v>0.73169838553975253</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A72" s="8">
         <v>3</v>
       </c>
-      <c r="B72" s="42">
+      <c r="B72" s="41">
         <f t="shared" si="0"/>
         <v>1.9952623149688797</v>
       </c>
@@ -6050,226 +6044,226 @@
         <v>0.69876661812551233</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="55" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="56"/>
-      <c r="C74" s="56"/>
-      <c r="D74" s="56"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="57"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="46" t="s">
+      <c r="B74" s="55"/>
+      <c r="C74" s="55"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="55"/>
+      <c r="F74" s="56"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B75" s="47" t="s">
+      <c r="B75" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="C75" s="47" t="s">
+      <c r="C75" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="D75" s="47" t="s">
+      <c r="D75" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="E75" s="47" t="s">
+      <c r="E75" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="F75" s="48" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B76" s="47" t="s">
+      <c r="F75" s="47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B76" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C76" s="47">
+      <c r="C76" s="46">
         <v>1</v>
       </c>
-      <c r="D76" s="47">
+      <c r="D76" s="46">
         <v>0.31</v>
       </c>
-      <c r="E76" s="49">
+      <c r="E76" s="48">
         <f>D76*C76</f>
         <v>0.31</v>
       </c>
-      <c r="F76" s="48" t="s">
+      <c r="F76" s="47" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="B77" s="47" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="47">
+      <c r="C77" s="46">
         <v>1</v>
       </c>
-      <c r="D77" s="47">
+      <c r="D77" s="46">
         <v>0.23</v>
       </c>
-      <c r="E77" s="49">
+      <c r="E77" s="48">
         <f>D77*C77</f>
         <v>0.23</v>
       </c>
-      <c r="F77" s="48" t="s">
+      <c r="F77" s="47" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="B78" s="47" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C78" s="47">
+      <c r="B78" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" s="46">
         <v>1</v>
       </c>
-      <c r="D78" s="47">
+      <c r="D78" s="46">
         <v>0.42</v>
       </c>
-      <c r="E78" s="49">
+      <c r="E78" s="48">
         <f t="shared" ref="E78:E83" si="1">D78*C78</f>
         <v>0.42</v>
       </c>
-      <c r="F78" s="48" t="s">
+      <c r="F78" s="47" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="46" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="B79" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="C79" s="47">
+      <c r="C79" s="46">
         <v>1</v>
       </c>
-      <c r="D79" s="47">
+      <c r="D79" s="46">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E79" s="49">
+      <c r="E79" s="48">
         <f t="shared" si="1"/>
         <v>0.28999999999999998</v>
       </c>
-      <c r="F79" s="48" t="s">
+      <c r="F79" s="47" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="B80" s="47"/>
-      <c r="C80" s="47">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" s="46"/>
+      <c r="C80" s="46">
         <v>1</v>
       </c>
-      <c r="D80" s="47">
+      <c r="D80" s="46">
         <v>0.69299999999999995</v>
       </c>
-      <c r="E80" s="49">
+      <c r="E80" s="48">
         <f t="shared" si="1"/>
         <v>0.69299999999999995</v>
       </c>
-      <c r="F80" s="48" t="s">
+      <c r="F80" s="47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A81" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" s="46" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="B81" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="C81" s="47">
+      <c r="C81" s="46">
         <v>1</v>
       </c>
-      <c r="D81" s="47">
+      <c r="D81" s="46">
         <v>1.1599999999999999</v>
       </c>
-      <c r="E81" s="49">
+      <c r="E81" s="48">
         <f t="shared" si="1"/>
         <v>1.1599999999999999</v>
       </c>
-      <c r="F81" s="48" t="s">
+      <c r="F81" s="47" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="B82" s="47" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A82" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C82" s="47">
+      <c r="B82" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C82" s="46">
         <v>1</v>
       </c>
-      <c r="D82" s="47">
+      <c r="D82" s="46">
         <v>0.1</v>
       </c>
-      <c r="E82" s="49">
+      <c r="E82" s="48">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F82" s="48" t="s">
+      <c r="F82" s="47" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="B83" s="47"/>
-      <c r="C83" s="47">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A83" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" s="46"/>
+      <c r="C83" s="46">
         <v>1</v>
       </c>
-      <c r="D83" s="47">
+      <c r="D83" s="46">
         <v>0.16</v>
       </c>
-      <c r="E83" s="53">
+      <c r="E83" s="52">
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-      <c r="F83" s="48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="46"/>
-      <c r="B84" s="47"/>
-      <c r="C84" s="47"/>
-      <c r="D84" s="47"/>
-      <c r="E84" s="47"/>
-      <c r="F84" s="48"/>
-    </row>
-    <row r="85" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="51"/>
+      <c r="F83" s="47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A84" s="45"/>
+      <c r="B84" s="46"/>
+      <c r="C84" s="46"/>
+      <c r="D84" s="46"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="47"/>
+    </row>
+    <row r="85" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A85" s="50"/>
       <c r="B85" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C85" s="9">
         <f>SUM(Table1[Quantity])</f>
         <v>8</v>
       </c>
       <c r="D85" s="9"/>
-      <c r="E85" s="54">
+      <c r="E85" s="53">
         <f>SUM(Table1[Price])</f>
         <v>3.363</v>
       </c>
-      <c r="F85" s="52"/>
+      <c r="F85" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>

<commit_message>
Updated buck converter calculation with new parts
</commit_message>
<xml_diff>
--- a/AOZ1281DI.xlsx
+++ b/AOZ1281DI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\SBC5-Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred\Downloads\SBC5-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42193EC4-010F-4369-826C-EE03C1A79576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84DEC69-6305-4FEE-B3A5-C23E9851B678}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19635" windowHeight="13875" activeTab="1" xr2:uid="{D55AB5B1-4BC1-429F-82B8-F59F2B41C856}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{D55AB5B1-4BC1-429F-82B8-F59F2B41C856}"/>
   </bookViews>
   <sheets>
     <sheet name="5V" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="97">
   <si>
     <t>R1</t>
   </si>
@@ -344,15 +344,6 @@
 (tan(delta))</t>
   </si>
   <si>
-    <t>1u</t>
-  </si>
-  <si>
-    <t>CC0603ZRY5V7BB105</t>
-  </si>
-  <si>
-    <t>NTE640</t>
-  </si>
-  <si>
     <t>Diode</t>
   </si>
   <si>
@@ -369,6 +360,15 @@
   </si>
   <si>
     <t>9.53k</t>
+  </si>
+  <si>
+    <t>CL21A106KOQNNNE</t>
+  </si>
+  <si>
+    <t>MBR230LSTR</t>
+  </si>
+  <si>
+    <t>500mV</t>
   </si>
 </sst>
 </file>
@@ -807,6 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -814,6 +815,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -834,13 +841,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -3338,7 +3338,7 @@
     <tableColumn id="1" xr3:uid="{CF3750E9-62E5-4A4E-A1A2-AC66A60CB49D}" name="Part number"/>
     <tableColumn id="2" xr3:uid="{9632C3C5-3C60-4B07-A1BE-20A4EABCF0CF}" name="Value"/>
     <tableColumn id="3" xr3:uid="{BE0EEA55-FC51-4E80-8ACA-578D9E3696A8}" name="Quantity"/>
-    <tableColumn id="4" xr3:uid="{EF27F1FA-C129-4822-A127-F216B7281EE2}" name="Price/unit"/>
+    <tableColumn id="4" xr3:uid="{EF27F1FA-C129-4822-A127-F216B7281EE2}" name="Price/unit" dataCellStyle="Currency"/>
     <tableColumn id="5" xr3:uid="{B4721B88-624D-4B67-890E-03CA1AA1958B}" name="Price" dataDxfId="8" dataCellStyle="Currency">
       <calculatedColumnFormula>D74*C74</calculatedColumnFormula>
     </tableColumn>
@@ -3355,7 +3355,7 @@
     <tableColumn id="1" xr3:uid="{4E26CB2C-D447-4F24-AF3E-EED540EF7026}" name="Part number"/>
     <tableColumn id="2" xr3:uid="{37C3BFF4-D988-49F4-90C8-412925F683D8}" name="Value"/>
     <tableColumn id="3" xr3:uid="{B54A28A7-C6D7-42A7-9475-6EAA259F41CE}" name="Quantity"/>
-    <tableColumn id="4" xr3:uid="{490048DC-F491-4B3B-9B4F-80E7EE88E6A1}" name="Price/unit"/>
+    <tableColumn id="4" xr3:uid="{490048DC-F491-4B3B-9B4F-80E7EE88E6A1}" name="Price/unit" dataCellStyle="Currency"/>
     <tableColumn id="5" xr3:uid="{44D7CBAB-E8E8-4CF5-B9B7-6D2EBA64816F}" name="Price" dataDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>D76*C76</calculatedColumnFormula>
     </tableColumn>
@@ -3665,47 +3665,47 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="56"/>
-    </row>
-    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="57"/>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>27</v>
       </c>
@@ -3718,15 +3718,15 @@
       <c r="D2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="E2" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="64"/>
+      <c r="F2" s="59"/>
       <c r="G2" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>0.8</v>
       </c>
@@ -3773,25 +3773,25 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A6" s="54" t="s">
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="56"/>
-    </row>
-    <row r="7" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="57"/>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>2</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23">
         <v>1E-3</v>
       </c>
@@ -3884,25 +3884,25 @@
         <v>4.2197137649303254E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A10" s="54" t="s">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="56"/>
-    </row>
-    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="57"/>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>2</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>1E-3</v>
       </c>
@@ -3995,20 +3995,20 @@
         <v>4.1991736713845696E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A14" s="54" t="s">
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
-      <c r="E14" s="54" t="s">
+      <c r="B14" s="56"/>
+      <c r="C14" s="57"/>
+      <c r="E14" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="56"/>
-    </row>
-    <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
+    </row>
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>41</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>0.01</v>
       </c>
@@ -4053,20 +4053,20 @@
         <v>0.49300664859163462</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="54" t="s">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="56"/>
-      <c r="E18" s="54" t="s">
+      <c r="B18" s="56"/>
+      <c r="C18" s="57"/>
+      <c r="E18" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="55"/>
-      <c r="G18" s="56"/>
-    </row>
-    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="F18" s="56"/>
+      <c r="G18" s="57"/>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>47</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>0.01</v>
       </c>
@@ -4110,18 +4110,18 @@
         <v>1.0055239898989898</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="60" t="s">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="62"/>
-    </row>
-    <row r="23" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="65"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>48</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
         <v>0.01</v>
       </c>
@@ -4165,18 +4165,18 @@
         <v>5.01</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="60" t="s">
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="62"/>
-    </row>
-    <row r="27" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="65"/>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>50</v>
       </c>
@@ -4196,20 +4196,20 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37">
-        <v>9.9999999999999995E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="B28" s="38">
-        <v>0.125</v>
+        <v>0.05</v>
       </c>
       <c r="C28" s="39">
         <f>B28/(2*PI()*E4*A28)</f>
-        <v>1.6578639905405763E-2</v>
+        <v>6.6314559621623065E-4</v>
       </c>
       <c r="D28" s="21">
         <f>F20*(C28+1/(8*E4*A28))</f>
-        <v>1.3339917077091336E-3</v>
+        <v>1.2240954204573905E-4</v>
       </c>
       <c r="E28" s="21">
         <f>F20/SQRT(12)</f>
@@ -4217,21 +4217,21 @@
       </c>
       <c r="F28" s="36">
         <f>D28+J12</f>
-        <v>4.9985973621085407</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" s="54" t="s">
+        <v>4.9973857799428769</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="56"/>
-    </row>
-    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57"/>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>53</v>
       </c>
@@ -4251,12 +4251,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>0.5</v>
       </c>
       <c r="B32" s="16">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C32" s="16">
         <v>2</v>
@@ -4273,14 +4273,14 @@
         <v>32.800000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="54" t="s">
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="56"/>
-    </row>
-    <row r="35" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B34" s="57"/>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>59</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <v>0.38</v>
       </c>
@@ -4297,19 +4297,19 @@
         <v>0.42263081060167651</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="54" t="s">
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="56"/>
-    </row>
-    <row r="39" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>61</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <f>0.38+(C4-3.3)*(0.24-0.38)/(12-3.3)</f>
         <v>0.24</v>
@@ -4360,16 +4360,16 @@
         <v>14.336236124263467</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A42" s="54" t="s">
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="56"/>
-    </row>
-    <row r="43" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="57"/>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
         <v>66</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="43">
         <f>E40+B36+E32+M12</f>
         <v>1.0937095665917871</v>
@@ -4401,20 +4401,20 @@
         <v>0.50780913054931565</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" s="54" t="s">
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="55"/>
-      <c r="C46" s="56"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="57"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
         <v>12</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="4"/>
       <c r="C48" s="7">
@@ -4434,7 +4434,7 @@
       </c>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>-20</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>0.68796144368040457</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>-19</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>0.72565841564890254</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>-18</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>0.75858913479286583</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>-17</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>0.78683314060841636</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>-16</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>0.81064772924535222</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>-15</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>0.83039908659056849</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>-14</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>0.8465025459682527</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>-13</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>0.85937615782215837</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>-12</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>0.86940784649076053</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>-11</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>0.87693418491977115</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>-10</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>0.88222794563366036</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>-9</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>0.88549159897513474</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>-8</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>0.88685439742453465</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>-7</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>0.88637132073878222</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>-6</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>0.88402281183909759</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>-5</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>0.87971485829539897</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>-4</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>0.87327957699602976</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>-3</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>0.86447707083421754</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>-2</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>0.85299996877927298</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>-1</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>0.8384827172270144</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>0</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>0.82051826483691459</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="8">
         <v>1</v>
       </c>
@@ -4699,20 +4699,20 @@
         <v>0.79868505756637986</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A72" s="57" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="58"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58"/>
-      <c r="E72" s="58"/>
-      <c r="F72" s="59"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B72" s="61"/>
+      <c r="C72" s="61"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="61"/>
+      <c r="F72" s="62"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="45" t="s">
         <v>70</v>
       </c>
@@ -4732,9 +4732,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A74" s="65" t="s">
-        <v>94</v>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="54" t="s">
+        <v>91</v>
       </c>
       <c r="B74" s="46" t="s">
         <v>77</v>
@@ -4742,7 +4742,7 @@
       <c r="C74" s="46">
         <v>1</v>
       </c>
-      <c r="D74" s="46">
+      <c r="D74" s="48">
         <v>0.31</v>
       </c>
       <c r="E74" s="48">
@@ -4753,17 +4753,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="45" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B75" s="46" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C75" s="46">
         <v>1</v>
       </c>
-      <c r="D75" s="46">
+      <c r="D75" s="48">
         <v>0.31</v>
       </c>
       <c r="E75" s="48">
@@ -4774,7 +4774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="49" t="s">
         <v>83</v>
       </c>
@@ -4784,7 +4784,7 @@
       <c r="C76" s="46">
         <v>1</v>
       </c>
-      <c r="D76" s="46">
+      <c r="D76" s="48">
         <v>0.42</v>
       </c>
       <c r="E76" s="48">
@@ -4795,7 +4795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="45" t="s">
         <v>80</v>
       </c>
@@ -4805,7 +4805,7 @@
       <c r="C77" s="46">
         <v>1</v>
       </c>
-      <c r="D77" s="46">
+      <c r="D77" s="48">
         <v>0.28999999999999998</v>
       </c>
       <c r="E77" s="48">
@@ -4816,7 +4816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="45" t="s">
         <v>84</v>
       </c>
@@ -4824,7 +4824,7 @@
       <c r="C78" s="46">
         <v>1</v>
       </c>
-      <c r="D78" s="46">
+      <c r="D78" s="48">
         <v>0.69299999999999995</v>
       </c>
       <c r="E78" s="48">
@@ -4835,9 +4835,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="45" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B79" s="46" t="s">
         <v>86</v>
@@ -4845,7 +4845,7 @@
       <c r="C79" s="46">
         <v>1</v>
       </c>
-      <c r="D79" s="46">
+      <c r="D79" s="48">
         <v>1.1599999999999999</v>
       </c>
       <c r="E79" s="48">
@@ -4856,47 +4856,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="45" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B80" s="46" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C80" s="46">
         <v>1</v>
       </c>
-      <c r="D80" s="46">
-        <v>0.1</v>
+      <c r="D80" s="48">
+        <v>0.12</v>
       </c>
       <c r="E80" s="48">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="F80" s="47" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="B81" s="46"/>
+        <v>95</v>
+      </c>
+      <c r="B81" s="46" t="s">
+        <v>96</v>
+      </c>
       <c r="C81" s="46">
         <v>1</v>
       </c>
-      <c r="D81" s="46">
-        <v>0.16</v>
+      <c r="D81" s="48">
+        <v>0.33</v>
       </c>
       <c r="E81" s="52">
         <f t="shared" si="1"/>
-        <v>0.16</v>
+        <v>0.33</v>
       </c>
       <c r="F81" s="47" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="45"/>
       <c r="B82" s="46"/>
       <c r="C82" s="46"/>
@@ -4904,10 +4906,10 @@
       <c r="E82" s="46"/>
       <c r="F82" s="47"/>
     </row>
-    <row r="83" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="50"/>
       <c r="B83" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C83" s="9">
         <f>SUM(Table2[Quantity])</f>
@@ -4916,18 +4918,12 @@
       <c r="D83" s="9"/>
       <c r="E83" s="53">
         <f>SUM(Table2[Price])</f>
-        <v>3.4430000000000001</v>
+        <v>3.633</v>
       </c>
       <c r="F83" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A6:M6"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="A42:D42"/>
@@ -4938,6 +4934,12 @@
     <mergeCell ref="A30:F30"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
   </mergeCells>
   <conditionalFormatting sqref="G40">
     <cfRule type="colorScale" priority="1">
@@ -4986,47 +4988,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5CAF6-20E4-4B67-AE88-D57C6FEB2845}">
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="56"/>
-    </row>
-    <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="57"/>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>27</v>
       </c>
@@ -5039,15 +5041,15 @@
       <c r="D2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="E2" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="64"/>
+      <c r="F2" s="59"/>
       <c r="G2" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -5070,7 +5072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>0.8</v>
       </c>
@@ -5094,25 +5096,25 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A6" s="54" t="s">
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="56"/>
-    </row>
-    <row r="7" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="57"/>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>2</v>
       </c>
@@ -5153,7 +5155,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23">
         <v>1E-3</v>
       </c>
@@ -5205,25 +5207,25 @@
         <v>2.1558305473483194E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A10" s="54" t="s">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="56"/>
-    </row>
-    <row r="11" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="57"/>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>2</v>
       </c>
@@ -5264,7 +5266,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>1E-3</v>
       </c>
@@ -5316,20 +5318,20 @@
         <v>2.1742631296614928E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A14" s="54" t="s">
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
-      <c r="E14" s="54" t="s">
+      <c r="B14" s="56"/>
+      <c r="C14" s="57"/>
+      <c r="E14" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="56"/>
-    </row>
-    <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="F14" s="56"/>
+      <c r="G14" s="57"/>
+    </row>
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>41</v>
       </c>
@@ -5349,7 +5351,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>0.01</v>
       </c>
@@ -5374,20 +5376,20 @@
         <v>0.69039852495778764</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="54" t="s">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="56"/>
-      <c r="E18" s="54" t="s">
+      <c r="B18" s="56"/>
+      <c r="C18" s="57"/>
+      <c r="E18" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="55"/>
-      <c r="G18" s="56"/>
-    </row>
-    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="F18" s="56"/>
+      <c r="G18" s="57"/>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>47</v>
       </c>
@@ -5407,7 +5409,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>0.01</v>
       </c>
@@ -5431,18 +5433,18 @@
         <v>1.4998469065656568</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="60" t="s">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="62"/>
-    </row>
-    <row r="23" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="65"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>48</v>
       </c>
@@ -5462,7 +5464,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
         <v>0.01</v>
       </c>
@@ -5486,18 +5488,18 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="60" t="s">
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="62"/>
-    </row>
-    <row r="27" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="65"/>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>50</v>
       </c>
@@ -5517,20 +5519,20 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37">
-        <v>9.9999999999999995E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="B28" s="44">
-        <v>0.125</v>
+        <v>0.05</v>
       </c>
       <c r="C28" s="39">
         <f>B28/(2*PI()*E4*A28)</f>
-        <v>1.6578639905405763E-2</v>
+        <v>6.6314559621623065E-4</v>
       </c>
       <c r="D28" s="21">
         <f>F20*(C28+1/(8*E4*A28))</f>
-        <v>1.1704824383927856E-3</v>
+        <v>1.0740562960641848E-4</v>
       </c>
       <c r="E28" s="21">
         <f>F20/SQRT(12)</f>
@@ -5538,21 +5540,21 @@
       </c>
       <c r="F28" s="36">
         <f>D28+J12</f>
-        <v>3.7208726663741536</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" s="54" t="s">
+        <v>3.7198095895653669</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="56"/>
-    </row>
-    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57"/>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>53</v>
       </c>
@@ -5572,12 +5574,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>0.5</v>
       </c>
       <c r="B32" s="16">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C32" s="16">
         <v>2</v>
@@ -5594,14 +5596,14 @@
         <v>49.036000000000008</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="54" t="s">
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="56"/>
-    </row>
-    <row r="35" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B34" s="57"/>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
         <v>59</v>
       </c>
@@ -5609,7 +5611,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <v>0.315</v>
       </c>
@@ -5618,19 +5620,19 @@
         <v>0.77946586749612856</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="54" t="s">
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="56"/>
-    </row>
-    <row r="39" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>61</v>
       </c>
@@ -5653,7 +5655,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
         <f>0.38+(C4-3.3)*(0.24-0.38)/(12-3.3)</f>
         <v>0.24</v>
@@ -5681,16 +5683,16 @@
         <v>30.683937809376324</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A42" s="54" t="s">
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="56"/>
-    </row>
-    <row r="43" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="57"/>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
         <v>66</v>
       </c>
@@ -5704,7 +5706,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="43">
         <f>E40+B36+E32+M12</f>
         <v>1.9505230721613918</v>
@@ -5722,20 +5724,20 @@
         <v>0.62350192268011606</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" s="54" t="s">
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="55"/>
-      <c r="C46" s="56"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="57"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
         <v>12</v>
       </c>
@@ -5746,7 +5748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="4"/>
       <c r="C48" s="7">
@@ -5755,7 +5757,7 @@
       </c>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>-20</v>
       </c>
@@ -5768,7 +5770,7 @@
         <v>0.62240619702935862</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>-19</v>
       </c>
@@ -5780,7 +5782,7 @@
         <v>0.66412682063428197</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>-18</v>
       </c>
@@ -5792,7 +5794,7 @@
         <v>0.70138296650231557</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>-17</v>
       </c>
@@ -5804,7 +5806,7 @@
         <v>0.73396499657999337</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>-16</v>
       </c>
@@ -5816,7 +5818,7 @@
         <v>0.76191025850561611</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>-15</v>
       </c>
@@ -5828,7 +5830,7 @@
         <v>0.78543698075365709</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>-14</v>
       </c>
@@ -5840,7 +5842,7 @@
         <v>0.80487597113032094</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>-13</v>
       </c>
@@ -5852,7 +5854,7 @@
         <v>0.82061010469092444</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>-12</v>
       </c>
@@ -5864,7 +5866,7 @@
         <v>0.83302635349491971</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>-11</v>
       </c>
@@ -5876,7 +5878,7 @@
         <v>0.8424810761986421</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>-10</v>
       </c>
@@ -5888,7 +5890,7 @@
         <v>0.84927688713019533</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>-9</v>
       </c>
@@ -5900,7 +5902,7 @@
         <v>0.85364843514519362</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>-8</v>
       </c>
@@ -5912,7 +5914,7 @@
         <v>0.85575438106203394</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>-7</v>
       </c>
@@ -5924,7 +5926,7 @@
         <v>0.85567334030054398</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>-6</v>
       </c>
@@ -5936,7 +5938,7 @@
         <v>0.85340226119018003</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>-5</v>
       </c>
@@ -5948,7 +5950,7 @@
         <v>0.84885648322503338</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>-4</v>
       </c>
@@ -5960,7 +5962,7 @@
         <v>0.84187150452944892</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>-3</v>
       </c>
@@ -5972,7 +5974,7 @@
         <v>0.83220727263234118</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>-2</v>
       </c>
@@ -5984,7 +5986,7 @@
         <v>0.81955658418054633</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>-1</v>
       </c>
@@ -5996,7 +5998,7 @@
         <v>0.80355987310932908</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>0</v>
       </c>
@@ -6008,7 +6010,7 @@
         <v>0.78382911787222842</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>1</v>
       </c>
@@ -6020,7 +6022,7 @@
         <v>0.75998350232147471</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>2</v>
       </c>
@@ -6032,7 +6034,7 @@
         <v>0.73169838553975253</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8">
         <v>3</v>
       </c>
@@ -6044,20 +6046,20 @@
         <v>0.69876661812551233</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A74" s="54" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="55"/>
-      <c r="C74" s="55"/>
-      <c r="D74" s="55"/>
-      <c r="E74" s="55"/>
-      <c r="F74" s="56"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B74" s="56"/>
+      <c r="C74" s="56"/>
+      <c r="D74" s="56"/>
+      <c r="E74" s="56"/>
+      <c r="F74" s="57"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="45" t="s">
         <v>70</v>
       </c>
@@ -6077,9 +6079,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A76" s="65" t="s">
-        <v>94</v>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="54" t="s">
+        <v>91</v>
       </c>
       <c r="B76" s="46" t="s">
         <v>77</v>
@@ -6087,7 +6089,7 @@
       <c r="C76" s="46">
         <v>1</v>
       </c>
-      <c r="D76" s="46">
+      <c r="D76" s="48">
         <v>0.31</v>
       </c>
       <c r="E76" s="48">
@@ -6098,7 +6100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="45" t="s">
         <v>78</v>
       </c>
@@ -6108,7 +6110,7 @@
       <c r="C77" s="46">
         <v>1</v>
       </c>
-      <c r="D77" s="46">
+      <c r="D77" s="48">
         <v>0.23</v>
       </c>
       <c r="E77" s="48">
@@ -6119,7 +6121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
         <v>83</v>
       </c>
@@ -6129,7 +6131,7 @@
       <c r="C78" s="46">
         <v>1</v>
       </c>
-      <c r="D78" s="46">
+      <c r="D78" s="48">
         <v>0.42</v>
       </c>
       <c r="E78" s="48">
@@ -6140,7 +6142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="45" t="s">
         <v>80</v>
       </c>
@@ -6150,7 +6152,7 @@
       <c r="C79" s="46">
         <v>1</v>
       </c>
-      <c r="D79" s="46">
+      <c r="D79" s="48">
         <v>0.28999999999999998</v>
       </c>
       <c r="E79" s="48">
@@ -6161,7 +6163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="45" t="s">
         <v>84</v>
       </c>
@@ -6169,7 +6171,7 @@
       <c r="C80" s="46">
         <v>1</v>
       </c>
-      <c r="D80" s="46">
+      <c r="D80" s="48">
         <v>0.69299999999999995</v>
       </c>
       <c r="E80" s="48">
@@ -6180,9 +6182,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="45" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B81" s="46" t="s">
         <v>86</v>
@@ -6190,7 +6192,7 @@
       <c r="C81" s="46">
         <v>1</v>
       </c>
-      <c r="D81" s="46">
+      <c r="D81" s="48">
         <v>1.1599999999999999</v>
       </c>
       <c r="E81" s="48">
@@ -6201,47 +6203,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="45" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B82" s="46" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C82" s="46">
         <v>1</v>
       </c>
-      <c r="D82" s="46">
-        <v>0.1</v>
+      <c r="D82" s="48">
+        <v>0.12</v>
       </c>
       <c r="E82" s="48">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="F82" s="47" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="B83" s="46"/>
+        <v>95</v>
+      </c>
+      <c r="B83" s="46" t="s">
+        <v>96</v>
+      </c>
       <c r="C83" s="46">
         <v>1</v>
       </c>
-      <c r="D83" s="46">
-        <v>0.16</v>
+      <c r="D83" s="48">
+        <v>0.33</v>
       </c>
       <c r="E83" s="52">
         <f t="shared" si="1"/>
-        <v>0.16</v>
+        <v>0.33</v>
       </c>
       <c r="F83" s="47" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="45"/>
       <c r="B84" s="46"/>
       <c r="C84" s="46"/>
@@ -6249,10 +6253,10 @@
       <c r="E84" s="46"/>
       <c r="F84" s="47"/>
     </row>
-    <row r="85" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="50"/>
       <c r="B85" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C85" s="9">
         <f>SUM(Table1[Quantity])</f>
@@ -6261,17 +6265,12 @@
       <c r="D85" s="9"/>
       <c r="E85" s="53">
         <f>SUM(Table1[Price])</f>
-        <v>3.363</v>
+        <v>3.5529999999999999</v>
       </c>
       <c r="F85" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A74:F74"/>
@@ -6283,6 +6282,11 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="A34:B34"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
   </mergeCells>
   <conditionalFormatting sqref="G40">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
Added 3V3 buck converter
</commit_message>
<xml_diff>
--- a/AOZ1281DI.xlsx
+++ b/AOZ1281DI.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred\Downloads\SBC5-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84DEC69-6305-4FEE-B3A5-C23E9851B678}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB56111-4372-4991-A152-CD17079C241F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{D55AB5B1-4BC1-429F-82B8-F59F2B41C856}"/>
   </bookViews>
   <sheets>
     <sheet name="5V" sheetId="1" r:id="rId1"/>
     <sheet name="3V7" sheetId="2" r:id="rId2"/>
+    <sheet name="3V3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="97">
   <si>
     <t>R1</t>
   </si>
@@ -325,12 +326,6 @@
     <t>10u</t>
   </si>
   <si>
-    <t>100u</t>
-  </si>
-  <si>
-    <t>EEU-FM1H101</t>
-  </si>
-  <si>
     <t>AOZ1281DI</t>
   </si>
   <si>
@@ -369,6 +364,12 @@
   </si>
   <si>
     <t>500mV</t>
+  </si>
+  <si>
+    <t>16k</t>
+  </si>
+  <si>
+    <t>RMCF0603FT16K0</t>
   </si>
 </sst>
 </file>
@@ -736,7 +737,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -802,12 +803,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -815,12 +821,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -841,6 +841,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -849,37 +855,90 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="24">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -944,6 +1003,68 @@
     <dxf>
       <border outline="0">
         <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
           <color indexed="64"/>
         </left>
         <right style="medium">
@@ -956,48 +1077,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2133,6 +2212,573 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Converter</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> efficiency</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'3V3'!$B$49:$B$72</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2589254117941664E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5848931924611124E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9952623149688792E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.511886431509578E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1622776601683784E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9810717055349727E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0118723362727206E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.3095734448019317E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.9432823472428096E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.12589254117941667</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15848931924611132</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.19952623149688795</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25118864315095801</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.31622776601683794</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.3981071705534972</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.50118723362727224</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.63095734448019325</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.79432823472428149</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.2589254117941673</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.5848931924611136</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.9952623149688797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'3V3'!$C$49:$C$72</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.59578607412179208</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.63872216746454036</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67740736624075792</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71150809415891203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74095778606822471</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.76589658875390043</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.78660297107672672</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.80342937743270559</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81674877066109941</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.82691430949605194</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.83423134821864409</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.83893943602332588</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.84120163497250633</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.84109881375795825</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.83862726105884511</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.83369878880873438</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8261433635025377</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.81571516999636562</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.80210383171876265</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.78495317758155125</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.76389023925664745</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.73856672208597696</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.70871356038854971</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.67420596628980245</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7B94-4877-849A-0E508FF86EDA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="411188808"/>
+        <c:axId val="411186512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="411188808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Current</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (A)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411186512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="411186512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Efficiency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="411188808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2213,6 +2859,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2730,6 +3416,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3331,15 +4533,58 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACD876C7-775A-4265-B4F4-CE07BC320D73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CFC006DC-B008-4A4E-AA27-302B054904D9}" name="Table2" displayName="Table2" ref="A73:F81" totalsRowShown="0" tableBorderDxfId="9">
-  <autoFilter ref="A73:F81" xr:uid="{4A76F8AC-30FC-48AB-B944-DEC569310B19}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CFC006DC-B008-4A4E-AA27-302B054904D9}" name="Table2" displayName="Table2" ref="A73:F80" totalsRowShown="0" tableBorderDxfId="23">
+  <autoFilter ref="A73:F80" xr:uid="{4A76F8AC-30FC-48AB-B944-DEC569310B19}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CF3750E9-62E5-4A4E-A1A2-AC66A60CB49D}" name="Part number"/>
     <tableColumn id="2" xr3:uid="{9632C3C5-3C60-4B07-A1BE-20A4EABCF0CF}" name="Value"/>
     <tableColumn id="3" xr3:uid="{BE0EEA55-FC51-4E80-8ACA-578D9E3696A8}" name="Quantity"/>
     <tableColumn id="4" xr3:uid="{EF27F1FA-C129-4822-A127-F216B7281EE2}" name="Price/unit" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{B4721B88-624D-4B67-890E-03CA1AA1958B}" name="Price" dataDxfId="8" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{B4721B88-624D-4B67-890E-03CA1AA1958B}" name="Price" dataDxfId="22" dataCellStyle="Currency">
       <calculatedColumnFormula>D74*C74</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{9A72E529-A5B4-4DCF-A857-F53DDAC6CE49}" name="Purpose"/>
@@ -3349,17 +4594,34 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F14AC3C4-D3B0-4392-B28C-49333C198959}" name="Table1" displayName="Table1" ref="A75:F83" totalsRowShown="0" tableBorderDxfId="1">
-  <autoFilter ref="A75:F83" xr:uid="{EB5E68EE-CBD9-4C56-AA00-C93F9EBD892A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F14AC3C4-D3B0-4392-B28C-49333C198959}" name="Table1" displayName="Table1" ref="A75:F82" totalsRowShown="0" tableBorderDxfId="21">
+  <autoFilter ref="A75:F82" xr:uid="{EB5E68EE-CBD9-4C56-AA00-C93F9EBD892A}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{4E26CB2C-D447-4F24-AF3E-EED540EF7026}" name="Part number"/>
     <tableColumn id="2" xr3:uid="{37C3BFF4-D988-49F4-90C8-412925F683D8}" name="Value"/>
     <tableColumn id="3" xr3:uid="{B54A28A7-C6D7-42A7-9475-6EAA259F41CE}" name="Quantity"/>
     <tableColumn id="4" xr3:uid="{490048DC-F491-4B3B-9B4F-80E7EE88E6A1}" name="Price/unit" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{44D7CBAB-E8E8-4CF5-B9B7-6D2EBA64816F}" name="Price" dataDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{44D7CBAB-E8E8-4CF5-B9B7-6D2EBA64816F}" name="Price" dataDxfId="20" dataCellStyle="Currency">
       <calculatedColumnFormula>D76*C76</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{957B4911-2007-4EAD-A0FF-C82F5429E22B}" name="Purpose"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F7DD0DAA-3162-4C0C-8D8B-D6455FF7B38A}" name="Table14" displayName="Table14" ref="A75:F82" totalsRowShown="0" tableBorderDxfId="19">
+  <autoFilter ref="A75:F82" xr:uid="{EB5E68EE-CBD9-4C56-AA00-C93F9EBD892A}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{406AF1D0-F757-479E-9805-BAFEB4AF475F}" name="Part number"/>
+    <tableColumn id="2" xr3:uid="{2F363E85-BB91-4334-A4FB-824BCB24B42F}" name="Value"/>
+    <tableColumn id="3" xr3:uid="{7462BA53-93B8-4332-B67F-B3068793F6A3}" name="Quantity"/>
+    <tableColumn id="4" xr3:uid="{BB60F329-21F2-4758-9B89-3B0C82452C96}" name="Price/unit" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{4BF27B93-DB09-4DC5-A099-23C9310249BC}" name="Price" dataDxfId="18" dataCellStyle="Currency">
+      <calculatedColumnFormula>D76*C76</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{D2709E11-BEA6-41F9-BE6A-83E2C5421A38}" name="Purpose"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3663,10 +4925,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D213B6F2-6B73-4D3E-A725-031E596F7E06}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M83"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3695,15 +4957,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="57"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -3718,10 +4980,10 @@
       <c r="D2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="59"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="29" t="s">
         <v>10</v>
       </c>
@@ -3775,21 +5037,21 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="58"/>
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
@@ -3886,21 +5148,21 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="57"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="58"/>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
@@ -3997,16 +5259,16 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="57"/>
-      <c r="E14" s="55" t="s">
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="E14" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="58"/>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
@@ -4055,16 +5317,16 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
-      <c r="E18" s="55" t="s">
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="E18" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="58"/>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
@@ -4112,21 +5374,21 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="65"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="64"/>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>49</v>
@@ -4167,21 +5429,21 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="63" t="s">
+      <c r="A26" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="65"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="64"/>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>49</v>
@@ -4222,14 +5484,14 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="58"/>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
@@ -4275,10 +5537,10 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="55" t="s">
+      <c r="A34" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="57"/>
+      <c r="B34" s="58"/>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
@@ -4299,15 +5561,15 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="55" t="s">
+      <c r="A38" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="57"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="58"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
@@ -4362,12 +5624,12 @@
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="55" t="s">
+      <c r="A42" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="57"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="58"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
@@ -4403,11 +5665,11 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="55" t="s">
+      <c r="A46" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="56"/>
-      <c r="C46" s="57"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="58"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -4703,14 +5965,14 @@
       <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="60" t="s">
+      <c r="A72" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="61"/>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="62"/>
+      <c r="B72" s="60"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="61"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="45" t="s">
@@ -4733,8 +5995,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="54" t="s">
-        <v>91</v>
+      <c r="A74" s="53" t="s">
+        <v>89</v>
       </c>
       <c r="B74" s="46" t="s">
         <v>77</v>
@@ -4755,10 +6017,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B75" s="46" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C75" s="46">
         <v>1</v>
@@ -4775,21 +6037,21 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="49" t="s">
-        <v>83</v>
+      <c r="A76" s="45" t="s">
+        <v>80</v>
       </c>
       <c r="B76" s="46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C76" s="46">
         <v>1</v>
       </c>
       <c r="D76" s="48">
-        <v>0.42</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E76" s="48">
-        <f t="shared" ref="E76:E81" si="1">D76*C76</f>
-        <v>0.42</v>
+        <f t="shared" ref="E76:E80" si="1">D76*C76</f>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F76" s="47" t="s">
         <v>6</v>
@@ -4797,133 +6059,118 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="B77" s="46" t="s">
-        <v>81</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B77" s="46"/>
       <c r="C77" s="46">
         <v>1</v>
       </c>
       <c r="D77" s="48">
-        <v>0.28999999999999998</v>
+        <v>0.69299999999999995</v>
       </c>
       <c r="E77" s="48">
         <f t="shared" si="1"/>
-        <v>0.28999999999999998</v>
+        <v>0.69299999999999995</v>
       </c>
       <c r="F77" s="47" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="B78" s="46"/>
       <c r="C78" s="46">
         <v>1</v>
       </c>
       <c r="D78" s="48">
-        <v>0.69299999999999995</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="E78" s="48">
         <f t="shared" si="1"/>
-        <v>0.69299999999999995</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="F78" s="47" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="45" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B79" s="46" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C79" s="46">
         <v>1</v>
       </c>
       <c r="D79" s="48">
-        <v>1.1599999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="E79" s="48">
         <f t="shared" si="1"/>
-        <v>1.1599999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="F79" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B80" s="46" t="s">
         <v>94</v>
-      </c>
-      <c r="B80" s="46" t="s">
-        <v>81</v>
       </c>
       <c r="C80" s="46">
         <v>1</v>
       </c>
       <c r="D80" s="48">
-        <v>0.12</v>
-      </c>
-      <c r="E80" s="48">
-        <f t="shared" si="1"/>
-        <v>0.12</v>
-      </c>
-      <c r="F80" s="47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="B81" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="C81" s="46">
-        <v>1</v>
-      </c>
-      <c r="D81" s="48">
         <v>0.33</v>
       </c>
-      <c r="E81" s="52">
+      <c r="E80" s="51">
         <f t="shared" si="1"/>
         <v>0.33</v>
       </c>
-      <c r="F81" s="47" t="s">
+      <c r="F80" s="47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="45"/>
+      <c r="B81" s="46"/>
+      <c r="C81" s="46"/>
+      <c r="D81" s="46"/>
+      <c r="E81" s="46"/>
+      <c r="F81" s="47"/>
+    </row>
+    <row r="82" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="49"/>
+      <c r="B82" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="45"/>
-      <c r="B82" s="46"/>
-      <c r="C82" s="46"/>
-      <c r="D82" s="46"/>
-      <c r="E82" s="46"/>
-      <c r="F82" s="47"/>
-    </row>
-    <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="50"/>
-      <c r="B83" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C83" s="9">
+      <c r="C82" s="9">
         <f>SUM(Table2[Quantity])</f>
-        <v>8</v>
-      </c>
-      <c r="D83" s="9"/>
-      <c r="E83" s="53">
+        <v>7</v>
+      </c>
+      <c r="D82" s="9"/>
+      <c r="E82" s="52">
         <f>SUM(Table2[Price])</f>
-        <v>3.633</v>
-      </c>
-      <c r="F83" s="51"/>
+        <v>3.2130000000000001</v>
+      </c>
+      <c r="F82" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="A42:D42"/>
@@ -4934,12 +6181,6 @@
     <mergeCell ref="A30:F30"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A6:M6"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
   </mergeCells>
   <conditionalFormatting sqref="G40">
     <cfRule type="colorScale" priority="1">
@@ -4952,26 +6193,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>$G$20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="between">
       <formula>$G$20</formula>
       <formula>1.2*$G$20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="greaterThan">
       <formula>1.2*$G$20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="5" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>$F$28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="between">
       <formula>$F$28</formula>
       <formula>1.2*$F$28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="greaterThan">
       <formula>1.2*$F$28</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4986,10 +6227,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5CAF6-20E4-4B67-AE88-D57C6FEB2845}">
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:XFD78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5018,15 +6259,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="57"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -5041,10 +6282,10 @@
       <c r="D2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="59"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="29" t="s">
         <v>10</v>
       </c>
@@ -5098,21 +6339,21 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="58"/>
     </row>
     <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
@@ -5209,21 +6450,21 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="57"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="58"/>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
@@ -5320,16 +6561,16 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="57"/>
-      <c r="E14" s="55" t="s">
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="E14" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="58"/>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
@@ -5378,16 +6619,16 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
-      <c r="E18" s="55" t="s">
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="E18" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="58"/>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
@@ -5435,21 +6676,21 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="65"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="64"/>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>49</v>
@@ -5490,21 +6731,21 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="63" t="s">
+      <c r="A26" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="65"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="64"/>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>49</v>
@@ -5545,14 +6786,14 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="58"/>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
@@ -5598,10 +6839,10 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="55" t="s">
+      <c r="A34" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="57"/>
+      <c r="B34" s="58"/>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
@@ -5622,15 +6863,15 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="55" t="s">
+      <c r="A38" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="57"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="58"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
@@ -5685,12 +6926,12 @@
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="55" t="s">
+      <c r="A42" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="57"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="58"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
@@ -5726,11 +6967,11 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="55" t="s">
+      <c r="A46" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="56"/>
-      <c r="C46" s="57"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="58"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -6050,14 +7291,14 @@
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="55" t="s">
+      <c r="A74" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="56"/>
-      <c r="C74" s="56"/>
-      <c r="D74" s="56"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="57"/>
+      <c r="B74" s="57"/>
+      <c r="C74" s="57"/>
+      <c r="D74" s="57"/>
+      <c r="E74" s="57"/>
+      <c r="F74" s="58"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="45" t="s">
@@ -6080,8 +7321,8 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="54" t="s">
-        <v>91</v>
+      <c r="A76" s="53" t="s">
+        <v>89</v>
       </c>
       <c r="B76" s="46" t="s">
         <v>77</v>
@@ -6122,21 +7363,21 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="49" t="s">
-        <v>83</v>
+      <c r="A78" s="45" t="s">
+        <v>80</v>
       </c>
       <c r="B78" s="46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C78" s="46">
         <v>1</v>
       </c>
       <c r="D78" s="48">
-        <v>0.42</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E78" s="48">
-        <f t="shared" ref="E78:E83" si="1">D78*C78</f>
-        <v>0.42</v>
+        <f t="shared" ref="E78:E82" si="1">D78*C78</f>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F78" s="47" t="s">
         <v>6</v>
@@ -6144,133 +7385,117 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="B79" s="46" t="s">
-        <v>81</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B79" s="46"/>
       <c r="C79" s="46">
         <v>1</v>
       </c>
       <c r="D79" s="48">
-        <v>0.28999999999999998</v>
+        <v>0.69299999999999995</v>
       </c>
       <c r="E79" s="48">
         <f t="shared" si="1"/>
-        <v>0.28999999999999998</v>
+        <v>0.69299999999999995</v>
       </c>
       <c r="F79" s="47" t="s">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="B80" s="46"/>
       <c r="C80" s="46">
         <v>1</v>
       </c>
       <c r="D80" s="48">
-        <v>0.69299999999999995</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="E80" s="48">
         <f t="shared" si="1"/>
-        <v>0.69299999999999995</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="F80" s="47" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="45" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B81" s="46" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C81" s="46">
         <v>1</v>
       </c>
       <c r="D81" s="48">
-        <v>1.1599999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="E81" s="48">
         <f t="shared" si="1"/>
-        <v>1.1599999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="F81" s="47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82" s="46" t="s">
         <v>94</v>
-      </c>
-      <c r="B82" s="46" t="s">
-        <v>81</v>
       </c>
       <c r="C82" s="46">
         <v>1</v>
       </c>
       <c r="D82" s="48">
-        <v>0.12</v>
-      </c>
-      <c r="E82" s="48">
-        <f t="shared" si="1"/>
-        <v>0.12</v>
-      </c>
-      <c r="F82" s="47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="B83" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="C83" s="46">
-        <v>1</v>
-      </c>
-      <c r="D83" s="48">
         <v>0.33</v>
       </c>
-      <c r="E83" s="52">
+      <c r="E82" s="51">
         <f t="shared" si="1"/>
         <v>0.33</v>
       </c>
-      <c r="F83" s="47" t="s">
+      <c r="F82" s="47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="45"/>
+      <c r="B83" s="46"/>
+      <c r="C83" s="46"/>
+      <c r="D83" s="46"/>
+      <c r="E83" s="46"/>
+      <c r="F83" s="47"/>
+    </row>
+    <row r="84" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="49"/>
+      <c r="B84" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="45"/>
-      <c r="B84" s="46"/>
-      <c r="C84" s="46"/>
-      <c r="D84" s="46"/>
-      <c r="E84" s="46"/>
-      <c r="F84" s="47"/>
-    </row>
-    <row r="85" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="50"/>
-      <c r="B85" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C85" s="9">
+      <c r="C84" s="9">
         <f>SUM(Table1[Quantity])</f>
-        <v>8</v>
-      </c>
-      <c r="D85" s="9"/>
-      <c r="E85" s="53">
+        <v>7</v>
+      </c>
+      <c r="D84" s="9"/>
+      <c r="E84" s="52">
         <f>SUM(Table1[Price])</f>
-        <v>3.5529999999999999</v>
-      </c>
-      <c r="F85" s="51"/>
+        <v>3.133</v>
+      </c>
+      <c r="F84" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E14:G14"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A74:F74"/>
@@ -6282,8 +7507,1329 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="A22:F22"/>
     <mergeCell ref="A34:B34"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G40">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="127"/>
+        <color rgb="FF92D050"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="cellIs" dxfId="11" priority="5" stopIfTrue="1" operator="lessThanOrEqual">
+      <formula>$G$20</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="between">
+      <formula>$G$20</formula>
+      <formula>1.2*$G$20</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="greaterThan">
+      <formula>1.2*$G$20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="cellIs" dxfId="8" priority="20" stopIfTrue="1" operator="lessThanOrEqual">
+      <formula>$F$28</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="21" operator="between">
+      <formula>$F$28</formula>
+      <formula>1.2*$F$28</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="22" operator="greaterThan">
+      <formula>1.2*$F$28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7ADE7B0-5D79-4492-9369-A99074ACCD24}">
+  <dimension ref="A1:M84"/>
+  <sheetViews>
+    <sheetView topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:XFD78"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="58"/>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="66"/>
+      <c r="G2" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="B4" s="16">
+        <v>3.3</v>
+      </c>
+      <c r="C4" s="16">
+        <v>12</v>
+      </c>
+      <c r="D4" s="16">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16">
+        <v>1200000</v>
+      </c>
+      <c r="F4" s="16">
+        <v>1800000</v>
+      </c>
+      <c r="G4" s="26">
+        <f>F4*0.0000001</f>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="58"/>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="B8" s="16">
+        <v>49900</v>
+      </c>
+      <c r="C8" s="24">
+        <f>A4*B8/(B4-A4)</f>
+        <v>15968</v>
+      </c>
+      <c r="D8" s="11">
+        <f>B8*(1-A8)</f>
+        <v>49850.1</v>
+      </c>
+      <c r="E8" s="11">
+        <f>B8*(1+A8)</f>
+        <v>49949.899999999994</v>
+      </c>
+      <c r="F8" s="20">
+        <f>C8*(1-A8)</f>
+        <v>15952.031999999999</v>
+      </c>
+      <c r="G8" s="20">
+        <f>C8*(1+A8)</f>
+        <v>15983.967999999999</v>
+      </c>
+      <c r="H8" s="21">
+        <f>A4*(1+D8/G8)</f>
+        <v>3.2950049950049953</v>
+      </c>
+      <c r="I8" s="21">
+        <f>A4*(1+B8/C8)</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="J8" s="21">
+        <f>A4*(1+E8/F8)</f>
+        <v>3.3050050050050048</v>
+      </c>
+      <c r="K8" s="21">
+        <f>ABS(MAX(J8, H8)-B4)</f>
+        <v>5.0050050050050032E-3</v>
+      </c>
+      <c r="L8" s="25">
+        <f>K8/B4</f>
+        <v>1.5166681833348496E-3</v>
+      </c>
+      <c r="M8" s="35">
+        <f>J8^2/(E8+F8)</f>
+        <v>1.6574716023663966E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="58"/>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="23">
+        <v>1E-3</v>
+      </c>
+      <c r="B12" s="16">
+        <f>B8</f>
+        <v>49900</v>
+      </c>
+      <c r="C12" s="19">
+        <v>16000</v>
+      </c>
+      <c r="D12" s="11">
+        <f>B12*(1-A12)</f>
+        <v>49850.1</v>
+      </c>
+      <c r="E12" s="11">
+        <f>B12*(1+A12)</f>
+        <v>49949.899999999994</v>
+      </c>
+      <c r="F12" s="20">
+        <f>C12*(1-A12)</f>
+        <v>15984</v>
+      </c>
+      <c r="G12" s="20">
+        <f>C12*(1+A12)</f>
+        <v>16015.999999999998</v>
+      </c>
+      <c r="H12" s="21">
+        <f>A4*(1+D12/G12)</f>
+        <v>3.2900149850149853</v>
+      </c>
+      <c r="I12" s="21">
+        <f>A4*(1+B12/C12)</f>
+        <v>3.2950000000000004</v>
+      </c>
+      <c r="J12" s="21">
+        <f>A4*(1+E12/F12)</f>
+        <v>3.2999949949949952</v>
+      </c>
+      <c r="K12" s="21">
+        <f>ABS(MAX(J12, H12)-B4)</f>
+        <v>5.0050050046657191E-6</v>
+      </c>
+      <c r="L12" s="22">
+        <f>K12/B4</f>
+        <v>1.5166681832320361E-6</v>
+      </c>
+      <c r="M12" s="35">
+        <f>J12*J12/(E12+F12)</f>
+        <v>1.651649146644142E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="E14" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="57"/>
+      <c r="G14" s="58"/>
+    </row>
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="B16" s="17">
+        <f>(D4/(E4*A16))*(1-B4/C4)*(B4/C4)</f>
+        <v>1.6614583333333332E-5</v>
+      </c>
+      <c r="C16" s="36">
+        <f>D4*SQRT((B4/C4)*(1-B4/C4))</f>
+        <v>0.44651427748729378</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="18">
+        <v>1.1E-4</v>
+      </c>
+      <c r="F16" s="21">
+        <f>(D4/(E4*E16))*(1-B4/C4)*(B4/C4)</f>
+        <v>1.5104166666666666E-3</v>
+      </c>
+      <c r="G16" s="36">
+        <f>D4*SQRT((B4/C4)*(1-B4/C4))</f>
+        <v>0.44651427748729378</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="E18" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="57"/>
+      <c r="G18" s="58"/>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="B20" s="34">
+        <f>(B4/(E4*A20))*(1-B4/C4)</f>
+        <v>1.9937500000000001E-4</v>
+      </c>
+      <c r="C20" s="13">
+        <f>D4+A20/2</f>
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="E20" s="15">
+        <v>2.2000000000000001E-4</v>
+      </c>
+      <c r="F20" s="21">
+        <f>(B4/(E4*E20))*(1-B4/C4)</f>
+        <v>9.0625000000000011E-3</v>
+      </c>
+      <c r="G20" s="36">
+        <f>D4+F20/2</f>
+        <v>1.0045312500000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="64"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="B24" s="44">
+        <v>0.125</v>
+      </c>
+      <c r="C24" s="21">
+        <f>B24/(2*PI()*E4*A20/(8*E4*A24))</f>
+        <v>0.15915494309189535</v>
+      </c>
+      <c r="D24" s="11">
+        <f>A20/(8*E4*(A24-A20*C24))</f>
+        <v>1.2388330740707554E-7</v>
+      </c>
+      <c r="E24" s="21">
+        <f>A20/SQRT(12)</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="F24" s="13">
+        <f>A24+B4</f>
+        <v>3.3099999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="64"/>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="37">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="B28" s="44">
+        <v>0.05</v>
+      </c>
+      <c r="C28" s="39">
+        <f>B28/(2*PI()*E4*A28)</f>
+        <v>6.6314559621623065E-4</v>
+      </c>
+      <c r="D28" s="21">
+        <f>F20*(C28+1/(8*E4*A28))</f>
+        <v>1.0041079863237625E-4</v>
+      </c>
+      <c r="E28" s="21">
+        <f>F20/SQRT(12)</f>
+        <v>2.6161184072654923E-3</v>
+      </c>
+      <c r="F28" s="36">
+        <f>D28+J12</f>
+        <v>3.3000954057936274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="58"/>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="B32" s="16">
+        <v>30</v>
+      </c>
+      <c r="C32" s="16">
+        <v>2</v>
+      </c>
+      <c r="D32" s="16">
+        <v>80</v>
+      </c>
+      <c r="E32" s="21">
+        <f>D4*(1-G4)*A32</f>
+        <v>0.41000000000000003</v>
+      </c>
+      <c r="F32" s="13">
+        <f>E32*D32</f>
+        <v>32.800000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="58"/>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="15">
+        <v>0.315</v>
+      </c>
+      <c r="B36" s="36">
+        <f>1.1*G20^2*A36</f>
+        <v>0.34964727066650397</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="58"/>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="14">
+        <f>0.38+(C4-3.3)*(0.24-0.38)/(12-3.3)</f>
+        <v>0.24</v>
+      </c>
+      <c r="B40" s="21">
+        <f>G20^2*A40</f>
+        <v>0.24217992773437505</v>
+      </c>
+      <c r="C40" s="21">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D40" s="11">
+        <f>C40*C4</f>
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="E40" s="21">
+        <f>D40+B40</f>
+        <v>0.26017992773437504</v>
+      </c>
+      <c r="F40" s="11">
+        <v>55</v>
+      </c>
+      <c r="G40" s="13">
+        <f>F40*E40</f>
+        <v>14.309896025390627</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="58"/>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="43">
+        <f>E40+B36+E32+M12</f>
+        <v>1.0199923633155434</v>
+      </c>
+      <c r="B44" s="21">
+        <f>B4*D4+A44</f>
+        <v>4.319992363315543</v>
+      </c>
+      <c r="C44" s="12">
+        <f>B4*D4/B44</f>
+        <v>0.76389023925664745</v>
+      </c>
+      <c r="D44" s="36">
+        <f>B44/C4</f>
+        <v>0.35999936360962859</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="57"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="7">
+        <f>C44</f>
+        <v>0.76389023925664745</v>
+      </c>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>-20</v>
+      </c>
+      <c r="B49" s="40">
+        <f>10^(A49/10)</f>
+        <v>0.01</v>
+      </c>
+      <c r="C49" s="7">
+        <f t="dataTable" ref="C49:C72" dt2D="0" dtr="0" r1="D4"/>
+        <v>0.59578607412179208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>-19</v>
+      </c>
+      <c r="B50" s="40">
+        <f t="shared" ref="B50:B72" si="0">10^(A50/10)</f>
+        <v>1.2589254117941664E-2</v>
+      </c>
+      <c r="C50" s="7">
+        <v>0.63872216746454036</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <v>-18</v>
+      </c>
+      <c r="B51" s="40">
+        <f t="shared" si="0"/>
+        <v>1.5848931924611124E-2</v>
+      </c>
+      <c r="C51" s="7">
+        <v>0.67740736624075792</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>-17</v>
+      </c>
+      <c r="B52" s="40">
+        <f t="shared" si="0"/>
+        <v>1.9952623149688792E-2</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0.71150809415891203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <v>-16</v>
+      </c>
+      <c r="B53" s="40">
+        <f t="shared" si="0"/>
+        <v>2.511886431509578E-2</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0.74095778606822471</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <v>-15</v>
+      </c>
+      <c r="B54" s="40">
+        <f t="shared" si="0"/>
+        <v>3.1622776601683784E-2</v>
+      </c>
+      <c r="C54" s="7">
+        <v>0.76589658875390043</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
+        <v>-14</v>
+      </c>
+      <c r="B55" s="40">
+        <f t="shared" si="0"/>
+        <v>3.9810717055349727E-2</v>
+      </c>
+      <c r="C55" s="7">
+        <v>0.78660297107672672</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <v>-13</v>
+      </c>
+      <c r="B56" s="40">
+        <f t="shared" si="0"/>
+        <v>5.0118723362727206E-2</v>
+      </c>
+      <c r="C56" s="7">
+        <v>0.80342937743270559</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <v>-12</v>
+      </c>
+      <c r="B57" s="40">
+        <f t="shared" si="0"/>
+        <v>6.3095734448019317E-2</v>
+      </c>
+      <c r="C57" s="7">
+        <v>0.81674877066109941</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <v>-11</v>
+      </c>
+      <c r="B58" s="40">
+        <f t="shared" si="0"/>
+        <v>7.9432823472428096E-2</v>
+      </c>
+      <c r="C58" s="7">
+        <v>0.82691430949605194</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>-10</v>
+      </c>
+      <c r="B59" s="40">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="C59" s="7">
+        <v>0.83423134821864409</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>-9</v>
+      </c>
+      <c r="B60" s="40">
+        <f t="shared" si="0"/>
+        <v>0.12589254117941667</v>
+      </c>
+      <c r="C60" s="7">
+        <v>0.83893943602332588</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <v>-8</v>
+      </c>
+      <c r="B61" s="40">
+        <f t="shared" si="0"/>
+        <v>0.15848931924611132</v>
+      </c>
+      <c r="C61" s="7">
+        <v>0.84120163497250633</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <v>-7</v>
+      </c>
+      <c r="B62" s="40">
+        <f t="shared" si="0"/>
+        <v>0.19952623149688795</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0.84109881375795825</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="5">
+        <v>-6</v>
+      </c>
+      <c r="B63" s="40">
+        <f t="shared" si="0"/>
+        <v>0.25118864315095801</v>
+      </c>
+      <c r="C63" s="7">
+        <v>0.83862726105884511</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>-5</v>
+      </c>
+      <c r="B64" s="40">
+        <f t="shared" si="0"/>
+        <v>0.31622776601683794</v>
+      </c>
+      <c r="C64" s="7">
+        <v>0.83369878880873438</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>-4</v>
+      </c>
+      <c r="B65" s="40">
+        <f t="shared" si="0"/>
+        <v>0.3981071705534972</v>
+      </c>
+      <c r="C65" s="7">
+        <v>0.8261433635025377</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>-3</v>
+      </c>
+      <c r="B66" s="40">
+        <f t="shared" si="0"/>
+        <v>0.50118723362727224</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0.81571516999636562</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>-2</v>
+      </c>
+      <c r="B67" s="40">
+        <f t="shared" si="0"/>
+        <v>0.63095734448019325</v>
+      </c>
+      <c r="C67" s="7">
+        <v>0.80210383171876265</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <v>-1</v>
+      </c>
+      <c r="B68" s="40">
+        <f t="shared" si="0"/>
+        <v>0.79432823472428149</v>
+      </c>
+      <c r="C68" s="7">
+        <v>0.78495317758155125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
+        <v>0</v>
+      </c>
+      <c r="B69" s="40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C69" s="7">
+        <v>0.76389023925664745</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
+        <v>1</v>
+      </c>
+      <c r="B70" s="40">
+        <f t="shared" si="0"/>
+        <v>1.2589254117941673</v>
+      </c>
+      <c r="C70" s="7">
+        <v>0.73856672208597696</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>2</v>
+      </c>
+      <c r="B71" s="40">
+        <f t="shared" si="0"/>
+        <v>1.5848931924611136</v>
+      </c>
+      <c r="C71" s="7">
+        <v>0.70871356038854971</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="8">
+        <v>3</v>
+      </c>
+      <c r="B72" s="41">
+        <f t="shared" si="0"/>
+        <v>1.9952623149688797</v>
+      </c>
+      <c r="C72" s="10">
+        <v>0.67420596628980245</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B74" s="57"/>
+      <c r="C74" s="57"/>
+      <c r="D74" s="57"/>
+      <c r="E74" s="57"/>
+      <c r="F74" s="58"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="E75" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="F75" s="47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76" s="46">
+        <v>1</v>
+      </c>
+      <c r="D76" s="48">
+        <v>0.31</v>
+      </c>
+      <c r="E76" s="48">
+        <f>D76*C76</f>
+        <v>0.31</v>
+      </c>
+      <c r="F76" s="47" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B77" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C77" s="46">
+        <v>1</v>
+      </c>
+      <c r="D77" s="48">
+        <v>0.1</v>
+      </c>
+      <c r="E77" s="48">
+        <f>D77*C77</f>
+        <v>0.1</v>
+      </c>
+      <c r="F77" s="47" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" s="46">
+        <v>1</v>
+      </c>
+      <c r="D78" s="48">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E78" s="48">
+        <f t="shared" ref="E78:E82" si="1">D78*C78</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F78" s="47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" s="46"/>
+      <c r="C79" s="46">
+        <v>1</v>
+      </c>
+      <c r="D79" s="48">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="E79" s="48">
+        <f t="shared" si="1"/>
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="F79" s="47" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80" s="46">
+        <v>1</v>
+      </c>
+      <c r="D80" s="48">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E80" s="48">
+        <f t="shared" si="1"/>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F80" s="47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C81" s="46">
+        <v>1</v>
+      </c>
+      <c r="D81" s="48">
+        <v>0.12</v>
+      </c>
+      <c r="E81" s="48">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="F81" s="47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C82" s="46">
+        <v>1</v>
+      </c>
+      <c r="D82" s="48">
+        <v>0.33</v>
+      </c>
+      <c r="E82" s="51">
+        <f t="shared" si="1"/>
+        <v>0.33</v>
+      </c>
+      <c r="F82" s="47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="45"/>
+      <c r="B83" s="46"/>
+      <c r="C83" s="46"/>
+      <c r="D83" s="46"/>
+      <c r="E83" s="46"/>
+      <c r="F83" s="47"/>
+    </row>
+    <row r="84" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="49"/>
+      <c r="B84" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84" s="9">
+        <f>SUM(Table14[Quantity])</f>
+        <v>7</v>
+      </c>
+      <c r="D84" s="9"/>
+      <c r="E84" s="52">
+        <f>SUM(Table14[Price])</f>
+        <v>3.0030000000000001</v>
+      </c>
+      <c r="F84" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A74:F74"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A6:M6"/>
     <mergeCell ref="A10:M10"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="E14:G14"/>
@@ -6299,26 +8845,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>$G$20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="between">
       <formula>$G$20</formula>
       <formula>1.2*$G$20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>1.2*$G$20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="cellIs" dxfId="4" priority="20" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="5" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>$F$28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="21" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="between">
       <formula>$F$28</formula>
       <formula>1.2*$F$28</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="greaterThan">
       <formula>1.2*$F$28</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Replaced buck converter inductor
</commit_message>
<xml_diff>
--- a/AOZ1281DI.xlsx
+++ b/AOZ1281DI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred\Downloads\SBC5-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB56111-4372-4991-A152-CD17079C241F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A772FBDD-4DBD-46AC-8A5C-47592E5464AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{D55AB5B1-4BC1-429F-82B8-F59F2B41C856}"/>
   </bookViews>
@@ -332,9 +332,6 @@
     <t>Converter IC</t>
   </si>
   <si>
-    <t>220u</t>
-  </si>
-  <si>
     <t>Dissipation factor
 (tan(delta))</t>
   </si>
@@ -342,9 +339,6 @@
     <t>Diode</t>
   </si>
   <si>
-    <t>SRR1210-221M</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -370,6 +364,12 @@
   </si>
   <si>
     <t>RMCF0603FT16K0</t>
+  </si>
+  <si>
+    <t>22u</t>
+  </si>
+  <si>
+    <t>MPL-SE4030-220</t>
   </si>
 </sst>
 </file>
@@ -1268,70 +1268,70 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>0.68796144368040457</c:v>
+                  <c:v>0.67054019580611668</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.72565841564890254</c:v>
+                  <c:v>0.7093312481797559</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75858913479286583</c:v>
+                  <c:v>0.74343263398828474</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.78683314060841636</c:v>
+                  <c:v>0.77286275530858739</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81064772924535222</c:v>
+                  <c:v>0.7978376203866393</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.83039908659056849</c:v>
+                  <c:v>0.81870168698250434</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8465025459682527</c:v>
+                  <c:v>0.83586565033224858</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.85937615782215837</c:v>
+                  <c:v>0.84975675380187365</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.86940784649076053</c:v>
+                  <c:v>0.86078285856632686</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.87693418491977115</c:v>
+                  <c:v>0.86930881169528895</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.88222794563366036</c:v>
+                  <c:v>0.87564243255804097</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.88549159897513474</c:v>
+                  <c:v>0.88002723254079351</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.88685439742453465</c:v>
+                  <c:v>0.88263933259146488</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.88637132073878222</c:v>
+                  <c:v>0.8835866153945191</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.88402281183909759</c:v>
+                  <c:v>0.8829087553888666</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.87971485829539897</c:v>
+                  <c:v>0.88057733230263791</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.87327957699602976</c:v>
+                  <c:v>0.87649574427130561</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.86447707083421754</c:v>
+                  <c:v>0.87049912346163727</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.85299996877927298</c:v>
+                  <c:v>0.86235496107124121</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.8384827172270144</c:v>
+                  <c:v>0.85176570165384458</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.82051826483691459</c:v>
+                  <c:v>0.83837516890181252</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.79868505756637986</c:v>
+                  <c:v>0.8217812724818323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1828,76 +1828,76 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0.62240619702935862</c:v>
+                  <c:v>0.60694098098188809</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66412682063428197</c:v>
+                  <c:v>0.64918283747876848</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70138296650231557</c:v>
+                  <c:v>0.68709838768614917</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.73396499657999337</c:v>
+                  <c:v>0.72042339254414312</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.76191025850561611</c:v>
+                  <c:v>0.74915127999094144</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.78543698075365709</c:v>
+                  <c:v>0.77347013867809278</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.80487597113032094</c:v>
+                  <c:v>0.79369476344884471</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.82061010469092444</c:v>
+                  <c:v>0.81020478790060058</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.83302635349491971</c:v>
+                  <c:v>0.82339465618037966</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8424810761986421</c:v>
+                  <c:v>0.83363686584004326</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.84927688713019533</c:v>
+                  <c:v>0.84125718873795774</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.85364843514519362</c:v>
+                  <c:v>0.84651932267309327</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.85575438106203394</c:v>
+                  <c:v>0.84961620510478086</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.85567334030054398</c:v>
+                  <c:v>0.85066558479248222</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.85340226119018003</c:v>
+                  <c:v>0.84970807293942185</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.84885648322503338</c:v>
+                  <c:v>0.84670659921071656</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.84187150452944892</c:v>
+                  <c:v>0.84154690569827428</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.83220727263234118</c:v>
+                  <c:v>0.83403941368002998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.81955658418054633</c:v>
+                  <c:v>0.82392350535147041</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.80355987310932908</c:v>
+                  <c:v>0.81087596763098013</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.78382911787222842</c:v>
+                  <c:v>0.79452597745423481</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.75998350232147471</c:v>
+                  <c:v>0.77447939032118507</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.73169838553975253</c:v>
+                  <c:v>0.75035490832686869</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.69876661812551233</c:v>
+                  <c:v>0.721833507180207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2395,76 +2395,76 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0.59578607412179208</c:v>
+                  <c:v>0.58163651571793351</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63872216746454036</c:v>
+                  <c:v>0.62488429844581783</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67740736624075792</c:v>
+                  <c:v>0.66403091546442838</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.71150809415891203</c:v>
+                  <c:v>0.69869681740826572</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.74095778606822471</c:v>
+                  <c:v>0.72877631784384134</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.76589658875390043</c:v>
+                  <c:v>0.75438122805404573</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.78660297107672672</c:v>
+                  <c:v>0.77577383664316402</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.80342937743270559</c:v>
+                  <c:v>0.79330213327789811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.81674877066109941</c:v>
+                  <c:v>0.80734499658787695</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.82691430949605194</c:v>
+                  <c:v>0.8182702897843106</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.83423134821864409</c:v>
+                  <c:v>0.82640547618124327</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.83893943602332588</c:v>
+                  <c:v>0.83201860215341572</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.84120163497250633</c:v>
+                  <c:v>0.83530694466114208</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.84109881375795825</c:v>
+                  <c:v>0.8363908251939759</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.83862726105884511</c:v>
+                  <c:v>0.8353106794105708</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.83369878880873438</c:v>
+                  <c:v>0.832026210319598</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.8261433635025377</c:v>
+                  <c:v>0.82641723207764051</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.81571516999636562</c:v>
+                  <c:v>0.81828659597923215</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.80210383171876265</c:v>
+                  <c:v>0.80736636947044282</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.78495317758155125</c:v>
+                  <c:v>0.79332917772098455</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.76389023925664745</c:v>
+                  <c:v>0.77580720513426271</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.73856672208597696</c:v>
+                  <c:v>0.75442155983572612</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.70871356038854971</c:v>
+                  <c:v>0.72882415546272294</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.67420596628980245</c:v>
+                  <c:v>0.69875250239399345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4927,8 +4927,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5361,15 +5361,15 @@
         <v>1.0049999999999999</v>
       </c>
       <c r="E20" s="15">
-        <v>2.2000000000000001E-4</v>
+        <v>2.1999999999999999E-5</v>
       </c>
       <c r="F20" s="21">
         <f>(B4/(E4*E20))*(1-B4/C4)</f>
-        <v>1.1047979797979796E-2</v>
+        <v>0.11047979797979797</v>
       </c>
       <c r="G20" s="36">
         <f>D4+F20/2</f>
-        <v>1.0055239898989898</v>
+        <v>1.055239898989899</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5388,7 +5388,7 @@
         <v>48</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>49</v>
@@ -5443,7 +5443,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>49</v>
@@ -5471,15 +5471,15 @@
       </c>
       <c r="D28" s="21">
         <f>F20*(C28+1/(8*E4*A28))</f>
-        <v>1.2240954204573905E-4</v>
+        <v>1.2240954204573906E-3</v>
       </c>
       <c r="E28" s="21">
         <f>F20/SQRT(12)</f>
-        <v>3.1892770551825915E-3</v>
+        <v>3.1892770551825919E-2</v>
       </c>
       <c r="F28" s="36">
         <f>D28+J12</f>
-        <v>4.9973857799428769</v>
+        <v>4.9984874658212881</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5552,11 +5552,11 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
-        <v>0.38</v>
+        <v>0.219</v>
       </c>
       <c r="B36" s="36">
         <f>1.1*G20^2*A36</f>
-        <v>0.42263081060167651</v>
+        <v>0.26824967678082917</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5601,7 +5601,7 @@
       </c>
       <c r="B40" s="21">
         <f>G20^2*A40</f>
-        <v>0.24265883862297211</v>
+        <v>0.26724749866085096</v>
       </c>
       <c r="C40" s="11">
         <v>1.5E-3</v>
@@ -5612,14 +5612,14 @@
       </c>
       <c r="E40" s="21">
         <f>D40+B40</f>
-        <v>0.26065883862297212</v>
+        <v>0.28524749866085097</v>
       </c>
       <c r="F40" s="11">
         <v>55</v>
       </c>
       <c r="G40" s="13">
         <f>F40*E40</f>
-        <v>14.336236124263467</v>
+        <v>15.688612426346804</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5648,19 +5648,19 @@
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="43">
         <f>E40+B36+E32+M12</f>
-        <v>1.0937095665917871</v>
+        <v>0.96391709280881865</v>
       </c>
       <c r="B44" s="21">
         <f>B4*D4+A44</f>
-        <v>6.0937095665917873</v>
+        <v>5.9639170928088188</v>
       </c>
       <c r="C44" s="42">
         <f>B4*D4/B44</f>
-        <v>0.82051826483691459</v>
+        <v>0.83837516890181252</v>
       </c>
       <c r="D44" s="36">
         <f>B44/C4</f>
-        <v>0.50780913054931565</v>
+        <v>0.49699309106740158</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5692,7 +5692,7 @@
       <c r="B48" s="4"/>
       <c r="C48" s="7">
         <f>C44</f>
-        <v>0.82051826483691459</v>
+        <v>0.83837516890181252</v>
       </c>
       <c r="D48" s="3"/>
     </row>
@@ -5706,7 +5706,7 @@
       </c>
       <c r="C49" s="7">
         <f t="dataTable" ref="C49:C70" dt2D="0" dtr="0" r1="D4"/>
-        <v>0.68796144368040457</v>
+        <v>0.67054019580611668</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5718,7 +5718,7 @@
         <v>1.2589254117941664E-2</v>
       </c>
       <c r="C50" s="7">
-        <v>0.72565841564890254</v>
+        <v>0.7093312481797559</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5730,7 +5730,7 @@
         <v>1.5848931924611124E-2</v>
       </c>
       <c r="C51" s="7">
-        <v>0.75858913479286583</v>
+        <v>0.74343263398828474</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5742,7 +5742,7 @@
         <v>1.9952623149688792E-2</v>
       </c>
       <c r="C52" s="7">
-        <v>0.78683314060841636</v>
+        <v>0.77286275530858739</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5754,7 +5754,7 @@
         <v>2.511886431509578E-2</v>
       </c>
       <c r="C53" s="7">
-        <v>0.81064772924535222</v>
+        <v>0.7978376203866393</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5766,7 +5766,7 @@
         <v>3.1622776601683784E-2</v>
       </c>
       <c r="C54" s="7">
-        <v>0.83039908659056849</v>
+        <v>0.81870168698250434</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5778,7 +5778,7 @@
         <v>3.9810717055349727E-2</v>
       </c>
       <c r="C55" s="7">
-        <v>0.8465025459682527</v>
+        <v>0.83586565033224858</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -5790,7 +5790,7 @@
         <v>5.0118723362727206E-2</v>
       </c>
       <c r="C56" s="7">
-        <v>0.85937615782215837</v>
+        <v>0.84975675380187365</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -5802,7 +5802,7 @@
         <v>6.3095734448019317E-2</v>
       </c>
       <c r="C57" s="7">
-        <v>0.86940784649076053</v>
+        <v>0.86078285856632686</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -5814,7 +5814,7 @@
         <v>7.9432823472428096E-2</v>
       </c>
       <c r="C58" s="7">
-        <v>0.87693418491977115</v>
+        <v>0.86930881169528895</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -5826,7 +5826,7 @@
         <v>0.1</v>
       </c>
       <c r="C59" s="7">
-        <v>0.88222794563366036</v>
+        <v>0.87564243255804097</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -5838,7 +5838,7 @@
         <v>0.12589254117941667</v>
       </c>
       <c r="C60" s="7">
-        <v>0.88549159897513474</v>
+        <v>0.88002723254079351</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -5850,7 +5850,7 @@
         <v>0.15848931924611132</v>
       </c>
       <c r="C61" s="7">
-        <v>0.88685439742453465</v>
+        <v>0.88263933259146488</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -5862,7 +5862,7 @@
         <v>0.19952623149688795</v>
       </c>
       <c r="C62" s="7">
-        <v>0.88637132073878222</v>
+        <v>0.8835866153945191</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -5874,7 +5874,7 @@
         <v>0.25118864315095801</v>
       </c>
       <c r="C63" s="7">
-        <v>0.88402281183909759</v>
+        <v>0.8829087553888666</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -5886,7 +5886,7 @@
         <v>0.31622776601683794</v>
       </c>
       <c r="C64" s="7">
-        <v>0.87971485829539897</v>
+        <v>0.88057733230263791</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -5898,7 +5898,7 @@
         <v>0.3981071705534972</v>
       </c>
       <c r="C65" s="7">
-        <v>0.87327957699602976</v>
+        <v>0.87649574427130561</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -5910,7 +5910,7 @@
         <v>0.50118723362727224</v>
       </c>
       <c r="C66" s="7">
-        <v>0.86447707083421754</v>
+        <v>0.87049912346163727</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -5922,7 +5922,7 @@
         <v>0.63095734448019325</v>
       </c>
       <c r="C67" s="7">
-        <v>0.85299996877927298</v>
+        <v>0.86235496107124121</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -5934,7 +5934,7 @@
         <v>0.79432823472428149</v>
       </c>
       <c r="C68" s="7">
-        <v>0.8384827172270144</v>
+        <v>0.85176570165384458</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -5946,7 +5946,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="7">
-        <v>0.82051826483691459</v>
+        <v>0.83837516890181252</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5958,7 +5958,7 @@
         <v>1.2589254117941673</v>
       </c>
       <c r="C70" s="10">
-        <v>0.79868505756637986</v>
+        <v>0.8217812724818323</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5996,7 +5996,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B74" s="46" t="s">
         <v>77</v>
@@ -6017,10 +6017,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="45" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B75" s="46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C75" s="46">
         <v>1</v>
@@ -6078,20 +6078,20 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="45" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B78" s="46" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C78" s="46">
         <v>1</v>
       </c>
       <c r="D78" s="48">
-        <v>1.1599999999999999</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E78" s="48">
         <f t="shared" si="1"/>
-        <v>1.1599999999999999</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F78" s="47" t="s">
         <v>7</v>
@@ -6099,7 +6099,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B79" s="46" t="s">
         <v>81</v>
@@ -6120,10 +6120,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B80" s="46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C80" s="46">
         <v>1</v>
@@ -6136,7 +6136,7 @@
         <v>0.33</v>
       </c>
       <c r="F80" s="47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -6150,7 +6150,7 @@
     <row r="82" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="49"/>
       <c r="B82" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C82" s="9">
         <f>SUM(Table2[Quantity])</f>
@@ -6159,7 +6159,7 @@
       <c r="D82" s="9"/>
       <c r="E82" s="52">
         <f>SUM(Table2[Price])</f>
-        <v>3.2130000000000001</v>
+        <v>2.613</v>
       </c>
       <c r="F82" s="50"/>
     </row>
@@ -6229,8 +6229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB5CAF6-20E4-4B67-AE88-D57C6FEB2845}">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:XFD78"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6663,15 +6663,15 @@
         <v>1.5</v>
       </c>
       <c r="E20" s="15">
-        <v>2.2000000000000001E-4</v>
+        <v>2.1999999999999999E-5</v>
       </c>
       <c r="F20" s="21">
         <f>(B4/(E4*E20))*(1-B4/C4)</f>
-        <v>9.6938131313131313E-3</v>
+        <v>9.6938131313131323E-2</v>
       </c>
       <c r="G20" s="36">
         <f>D4+F20/2</f>
-        <v>1.4998469065656568</v>
+        <v>1.5434690656565657</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -6690,7 +6690,7 @@
         <v>48</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>49</v>
@@ -6745,7 +6745,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>49</v>
@@ -6773,15 +6773,15 @@
       </c>
       <c r="D28" s="21">
         <f>F20*(C28+1/(8*E4*A28))</f>
-        <v>1.0740562960641848E-4</v>
+        <v>1.0740562960641848E-3</v>
       </c>
       <c r="E28" s="21">
         <f>F20/SQRT(12)</f>
-        <v>2.7983628104187828E-3</v>
+        <v>2.7983628104187832E-2</v>
       </c>
       <c r="F28" s="36">
         <f>D28+J12</f>
-        <v>3.7198095895653669</v>
+        <v>3.720776240231825</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -6854,11 +6854,11 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
-        <v>0.315</v>
+        <v>0.219</v>
       </c>
       <c r="B36" s="36">
         <f>1.1*G20^2*A36</f>
-        <v>0.77946586749612856</v>
+        <v>0.57389528867427542</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -6903,7 +6903,7 @@
       </c>
       <c r="B40" s="21">
         <f>G20^2*A40</f>
-        <v>0.53988977835229679</v>
+        <v>0.57175122159330038</v>
       </c>
       <c r="C40" s="21">
         <v>1.5E-3</v>
@@ -6914,14 +6914,14 @@
       </c>
       <c r="E40" s="21">
         <f>D40+B40</f>
-        <v>0.55788977835229681</v>
+        <v>0.5897512215933004</v>
       </c>
       <c r="F40" s="11">
         <v>55</v>
       </c>
       <c r="G40" s="13">
         <f>F40*E40</f>
-        <v>30.683937809376324</v>
+        <v>32.436317187631523</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -6950,19 +6950,19 @@
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="43">
         <f>E40+B36+E32+M12</f>
-        <v>1.9505230721613918</v>
+        <v>1.776813936580542</v>
       </c>
       <c r="B44" s="21">
         <f>B4*D4+A44</f>
-        <v>7.4820230721613923</v>
+        <v>7.3083139365805421</v>
       </c>
       <c r="C44" s="12">
         <f>B4*D4/B44</f>
-        <v>0.73930539195758871</v>
+        <v>0.75687772145542398</v>
       </c>
       <c r="D44" s="36">
         <f>B44/C4</f>
-        <v>0.62350192268011606</v>
+        <v>0.60902616138171184</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -6994,7 +6994,7 @@
       <c r="B48" s="4"/>
       <c r="C48" s="7">
         <f>C44</f>
-        <v>0.73930539195758871</v>
+        <v>0.75687772145542398</v>
       </c>
       <c r="D48" s="3"/>
     </row>
@@ -7008,7 +7008,7 @@
       </c>
       <c r="C49" s="7">
         <f t="dataTable" ref="C49:C72" dt2D="0" dtr="0" r1="D4"/>
-        <v>0.62240619702935862</v>
+        <v>0.60694098098188809</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -7020,7 +7020,7 @@
         <v>1.2589254117941664E-2</v>
       </c>
       <c r="C50" s="7">
-        <v>0.66412682063428197</v>
+        <v>0.64918283747876848</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -7032,7 +7032,7 @@
         <v>1.5848931924611124E-2</v>
       </c>
       <c r="C51" s="7">
-        <v>0.70138296650231557</v>
+        <v>0.68709838768614917</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -7044,7 +7044,7 @@
         <v>1.9952623149688792E-2</v>
       </c>
       <c r="C52" s="7">
-        <v>0.73396499657999337</v>
+        <v>0.72042339254414312</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -7056,7 +7056,7 @@
         <v>2.511886431509578E-2</v>
       </c>
       <c r="C53" s="7">
-        <v>0.76191025850561611</v>
+        <v>0.74915127999094144</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -7068,7 +7068,7 @@
         <v>3.1622776601683784E-2</v>
       </c>
       <c r="C54" s="7">
-        <v>0.78543698075365709</v>
+        <v>0.77347013867809278</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -7080,7 +7080,7 @@
         <v>3.9810717055349727E-2</v>
       </c>
       <c r="C55" s="7">
-        <v>0.80487597113032094</v>
+        <v>0.79369476344884471</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -7092,7 +7092,7 @@
         <v>5.0118723362727206E-2</v>
       </c>
       <c r="C56" s="7">
-        <v>0.82061010469092444</v>
+        <v>0.81020478790060058</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -7104,7 +7104,7 @@
         <v>6.3095734448019317E-2</v>
       </c>
       <c r="C57" s="7">
-        <v>0.83302635349491971</v>
+        <v>0.82339465618037966</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -7116,7 +7116,7 @@
         <v>7.9432823472428096E-2</v>
       </c>
       <c r="C58" s="7">
-        <v>0.8424810761986421</v>
+        <v>0.83363686584004326</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -7128,7 +7128,7 @@
         <v>0.1</v>
       </c>
       <c r="C59" s="7">
-        <v>0.84927688713019533</v>
+        <v>0.84125718873795774</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -7140,7 +7140,7 @@
         <v>0.12589254117941667</v>
       </c>
       <c r="C60" s="7">
-        <v>0.85364843514519362</v>
+        <v>0.84651932267309327</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -7152,7 +7152,7 @@
         <v>0.15848931924611132</v>
       </c>
       <c r="C61" s="7">
-        <v>0.85575438106203394</v>
+        <v>0.84961620510478086</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -7164,7 +7164,7 @@
         <v>0.19952623149688795</v>
       </c>
       <c r="C62" s="7">
-        <v>0.85567334030054398</v>
+        <v>0.85066558479248222</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -7176,7 +7176,7 @@
         <v>0.25118864315095801</v>
       </c>
       <c r="C63" s="7">
-        <v>0.85340226119018003</v>
+        <v>0.84970807293942185</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -7188,7 +7188,7 @@
         <v>0.31622776601683794</v>
       </c>
       <c r="C64" s="7">
-        <v>0.84885648322503338</v>
+        <v>0.84670659921071656</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -7200,7 +7200,7 @@
         <v>0.3981071705534972</v>
       </c>
       <c r="C65" s="7">
-        <v>0.84187150452944892</v>
+        <v>0.84154690569827428</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -7212,7 +7212,7 @@
         <v>0.50118723362727224</v>
       </c>
       <c r="C66" s="7">
-        <v>0.83220727263234118</v>
+        <v>0.83403941368002998</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -7224,7 +7224,7 @@
         <v>0.63095734448019325</v>
       </c>
       <c r="C67" s="7">
-        <v>0.81955658418054633</v>
+        <v>0.82392350535147041</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -7236,7 +7236,7 @@
         <v>0.79432823472428149</v>
       </c>
       <c r="C68" s="7">
-        <v>0.80355987310932908</v>
+        <v>0.81087596763098013</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -7248,7 +7248,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="7">
-        <v>0.78382911787222842</v>
+        <v>0.79452597745423481</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -7260,7 +7260,7 @@
         <v>1.2589254117941673</v>
       </c>
       <c r="C70" s="7">
-        <v>0.75998350232147471</v>
+        <v>0.77447939032118507</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -7272,7 +7272,7 @@
         <v>1.5848931924611136</v>
       </c>
       <c r="C71" s="7">
-        <v>0.73169838553975253</v>
+        <v>0.75035490832686869</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7284,7 +7284,7 @@
         <v>1.9952623149688797</v>
       </c>
       <c r="C72" s="10">
-        <v>0.69876661812551233</v>
+        <v>0.721833507180207</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7322,7 +7322,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B76" s="46" t="s">
         <v>77</v>
@@ -7404,20 +7404,20 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="45" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B80" s="46" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C80" s="46">
         <v>1</v>
       </c>
       <c r="D80" s="48">
-        <v>1.1599999999999999</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E80" s="48">
         <f t="shared" si="1"/>
-        <v>1.1599999999999999</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F80" s="47" t="s">
         <v>7</v>
@@ -7425,7 +7425,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B81" s="46" t="s">
         <v>81</v>
@@ -7446,10 +7446,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B82" s="46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C82" s="46">
         <v>1</v>
@@ -7462,7 +7462,7 @@
         <v>0.33</v>
       </c>
       <c r="F82" s="47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -7476,7 +7476,7 @@
     <row r="84" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="49"/>
       <c r="B84" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C84" s="9">
         <f>SUM(Table1[Quantity])</f>
@@ -7485,7 +7485,7 @@
       <c r="D84" s="9"/>
       <c r="E84" s="52">
         <f>SUM(Table1[Price])</f>
-        <v>3.133</v>
+        <v>2.5330000000000004</v>
       </c>
       <c r="F84" s="50"/>
     </row>
@@ -7555,8 +7555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7ADE7B0-5D79-4492-9369-A99074ACCD24}">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:XFD78"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7989,15 +7989,15 @@
         <v>1.0049999999999999</v>
       </c>
       <c r="E20" s="15">
-        <v>2.2000000000000001E-4</v>
+        <v>2.1999999999999999E-5</v>
       </c>
       <c r="F20" s="21">
         <f>(B4/(E4*E20))*(1-B4/C4)</f>
-        <v>9.0625000000000011E-3</v>
+        <v>9.0625000000000011E-2</v>
       </c>
       <c r="G20" s="36">
         <f>D4+F20/2</f>
-        <v>1.0045312500000001</v>
+        <v>1.0453125000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -8016,7 +8016,7 @@
         <v>48</v>
       </c>
       <c r="B23" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="54" t="s">
         <v>49</v>
@@ -8071,7 +8071,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="54" t="s">
         <v>49</v>
@@ -8099,15 +8099,15 @@
       </c>
       <c r="D28" s="21">
         <f>F20*(C28+1/(8*E4*A28))</f>
-        <v>1.0041079863237625E-4</v>
+        <v>1.0041079863237626E-3</v>
       </c>
       <c r="E28" s="21">
         <f>F20/SQRT(12)</f>
-        <v>2.6161184072654923E-3</v>
+        <v>2.6161184072654921E-2</v>
       </c>
       <c r="F28" s="36">
         <f>D28+J12</f>
-        <v>3.3000954057936274</v>
+        <v>3.300999102981319</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -8180,11 +8180,11 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
-        <v>0.315</v>
+        <v>0.219</v>
       </c>
       <c r="B36" s="36">
         <f>1.1*G20^2*A36</f>
-        <v>0.34964727066650397</v>
+        <v>0.2632261838378907</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -8229,7 +8229,7 @@
       </c>
       <c r="B40" s="21">
         <f>G20^2*A40</f>
-        <v>0.24217992773437505</v>
+        <v>0.26224277343750002</v>
       </c>
       <c r="C40" s="21">
         <v>1.5E-3</v>
@@ -8240,14 +8240,14 @@
       </c>
       <c r="E40" s="21">
         <f>D40+B40</f>
-        <v>0.26017992773437504</v>
+        <v>0.28024277343750004</v>
       </c>
       <c r="F40" s="11">
         <v>55</v>
       </c>
       <c r="G40" s="13">
         <f>F40*E40</f>
-        <v>14.309896025390627</v>
+        <v>15.413352539062503</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -8276,19 +8276,19 @@
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="43">
         <f>E40+B36+E32+M12</f>
-        <v>1.0199923633155434</v>
+        <v>0.95363412219005528</v>
       </c>
       <c r="B44" s="21">
         <f>B4*D4+A44</f>
-        <v>4.319992363315543</v>
+        <v>4.2536341221900553</v>
       </c>
       <c r="C44" s="12">
         <f>B4*D4/B44</f>
-        <v>0.76389023925664745</v>
+        <v>0.77580720513426271</v>
       </c>
       <c r="D44" s="36">
         <f>B44/C4</f>
-        <v>0.35999936360962859</v>
+        <v>0.35446951018250461</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -8320,7 +8320,7 @@
       <c r="B48" s="4"/>
       <c r="C48" s="7">
         <f>C44</f>
-        <v>0.76389023925664745</v>
+        <v>0.77580720513426271</v>
       </c>
       <c r="D48" s="3"/>
     </row>
@@ -8334,7 +8334,7 @@
       </c>
       <c r="C49" s="7">
         <f t="dataTable" ref="C49:C72" dt2D="0" dtr="0" r1="D4"/>
-        <v>0.59578607412179208</v>
+        <v>0.58163651571793351</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -8346,7 +8346,7 @@
         <v>1.2589254117941664E-2</v>
       </c>
       <c r="C50" s="7">
-        <v>0.63872216746454036</v>
+        <v>0.62488429844581783</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -8358,7 +8358,7 @@
         <v>1.5848931924611124E-2</v>
       </c>
       <c r="C51" s="7">
-        <v>0.67740736624075792</v>
+        <v>0.66403091546442838</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -8370,7 +8370,7 @@
         <v>1.9952623149688792E-2</v>
       </c>
       <c r="C52" s="7">
-        <v>0.71150809415891203</v>
+        <v>0.69869681740826572</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -8382,7 +8382,7 @@
         <v>2.511886431509578E-2</v>
       </c>
       <c r="C53" s="7">
-        <v>0.74095778606822471</v>
+        <v>0.72877631784384134</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -8394,7 +8394,7 @@
         <v>3.1622776601683784E-2</v>
       </c>
       <c r="C54" s="7">
-        <v>0.76589658875390043</v>
+        <v>0.75438122805404573</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -8406,7 +8406,7 @@
         <v>3.9810717055349727E-2</v>
       </c>
       <c r="C55" s="7">
-        <v>0.78660297107672672</v>
+        <v>0.77577383664316402</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -8418,7 +8418,7 @@
         <v>5.0118723362727206E-2</v>
       </c>
       <c r="C56" s="7">
-        <v>0.80342937743270559</v>
+        <v>0.79330213327789811</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -8430,7 +8430,7 @@
         <v>6.3095734448019317E-2</v>
       </c>
       <c r="C57" s="7">
-        <v>0.81674877066109941</v>
+        <v>0.80734499658787695</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -8442,7 +8442,7 @@
         <v>7.9432823472428096E-2</v>
       </c>
       <c r="C58" s="7">
-        <v>0.82691430949605194</v>
+        <v>0.8182702897843106</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -8454,7 +8454,7 @@
         <v>0.1</v>
       </c>
       <c r="C59" s="7">
-        <v>0.83423134821864409</v>
+        <v>0.82640547618124327</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -8466,7 +8466,7 @@
         <v>0.12589254117941667</v>
       </c>
       <c r="C60" s="7">
-        <v>0.83893943602332588</v>
+        <v>0.83201860215341572</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -8478,7 +8478,7 @@
         <v>0.15848931924611132</v>
       </c>
       <c r="C61" s="7">
-        <v>0.84120163497250633</v>
+        <v>0.83530694466114208</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -8490,7 +8490,7 @@
         <v>0.19952623149688795</v>
       </c>
       <c r="C62" s="7">
-        <v>0.84109881375795825</v>
+        <v>0.8363908251939759</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -8502,7 +8502,7 @@
         <v>0.25118864315095801</v>
       </c>
       <c r="C63" s="7">
-        <v>0.83862726105884511</v>
+        <v>0.8353106794105708</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -8514,7 +8514,7 @@
         <v>0.31622776601683794</v>
       </c>
       <c r="C64" s="7">
-        <v>0.83369878880873438</v>
+        <v>0.832026210319598</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -8526,7 +8526,7 @@
         <v>0.3981071705534972</v>
       </c>
       <c r="C65" s="7">
-        <v>0.8261433635025377</v>
+        <v>0.82641723207764051</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -8538,7 +8538,7 @@
         <v>0.50118723362727224</v>
       </c>
       <c r="C66" s="7">
-        <v>0.81571516999636562</v>
+        <v>0.81828659597923215</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -8550,7 +8550,7 @@
         <v>0.63095734448019325</v>
       </c>
       <c r="C67" s="7">
-        <v>0.80210383171876265</v>
+        <v>0.80736636947044282</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -8562,7 +8562,7 @@
         <v>0.79432823472428149</v>
       </c>
       <c r="C68" s="7">
-        <v>0.78495317758155125</v>
+        <v>0.79332917772098455</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -8574,7 +8574,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="7">
-        <v>0.76389023925664745</v>
+        <v>0.77580720513426271</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -8586,7 +8586,7 @@
         <v>1.2589254117941673</v>
       </c>
       <c r="C70" s="7">
-        <v>0.73856672208597696</v>
+        <v>0.75442155983572612</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -8598,7 +8598,7 @@
         <v>1.5848931924611136</v>
       </c>
       <c r="C71" s="7">
-        <v>0.70871356038854971</v>
+        <v>0.72882415546272294</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8610,7 +8610,7 @@
         <v>1.9952623149688797</v>
       </c>
       <c r="C72" s="10">
-        <v>0.67420596628980245</v>
+        <v>0.69875250239399345</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8648,7 +8648,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B76" s="46" t="s">
         <v>77</v>
@@ -8669,10 +8669,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B77" s="46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C77" s="46">
         <v>1</v>
@@ -8730,20 +8730,20 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="45" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B80" s="46" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="C80" s="46">
         <v>1</v>
       </c>
       <c r="D80" s="48">
-        <v>1.1599999999999999</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E80" s="48">
         <f t="shared" si="1"/>
-        <v>1.1599999999999999</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F80" s="47" t="s">
         <v>7</v>
@@ -8751,7 +8751,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B81" s="46" t="s">
         <v>81</v>
@@ -8772,10 +8772,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B82" s="46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C82" s="46">
         <v>1</v>
@@ -8788,7 +8788,7 @@
         <v>0.33</v>
       </c>
       <c r="F82" s="47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -8802,7 +8802,7 @@
     <row r="84" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="49"/>
       <c r="B84" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C84" s="9">
         <f>SUM(Table14[Quantity])</f>
@@ -8811,7 +8811,7 @@
       <c r="D84" s="9"/>
       <c r="E84" s="52">
         <f>SUM(Table14[Price])</f>
-        <v>3.0030000000000001</v>
+        <v>2.403</v>
       </c>
       <c r="F84" s="50"/>
     </row>

</xml_diff>